<commit_message>
added notes legend logic
</commit_message>
<xml_diff>
--- a/src/supy/data_model/initial_states/parameter_analysis.xlsx
+++ b/src/supy/data_model/initial_states/parameter_analysis.xlsx
@@ -474,7 +474,11 @@
           <t>bldgs.icefrac</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr"/>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C2" t="inlineStr">
         <is>
           <t>SurfaceInitialState (state.py, 15)</t>
@@ -498,7 +502,11 @@
           <t>bldgs.snowdens</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr"/>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C3" t="inlineStr">
         <is>
           <t>SurfaceInitialState (state.py, 15)</t>
@@ -522,7 +530,11 @@
           <t>bldgs.snowfrac</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr"/>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C4" t="inlineStr">
         <is>
           <t>SurfaceInitialState (state.py, 15)</t>
@@ -546,7 +558,11 @@
           <t>bldgs.snowpack</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr"/>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C5" t="inlineStr">
         <is>
           <t>SurfaceInitialState (state.py, 15)</t>
@@ -570,7 +586,11 @@
           <t>bldgs.snowwater</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr"/>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C6" t="inlineStr">
         <is>
           <t>SurfaceInitialState (state.py, 15)</t>
@@ -642,7 +662,11 @@
           <t>bldgs.temperature</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr"/>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="C9" t="inlineStr">
         <is>
           <t>RefValue (type.py, 33); SurfaceInitialState (state.py, 15); validate_temperature (state.py, 82)</t>
@@ -666,7 +690,11 @@
           <t>bldgs.tin</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr"/>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="C10" t="inlineStr">
         <is>
           <t>SurfaceInitialState (state.py, 15)</t>
@@ -690,7 +718,11 @@
           <t>bldgs.tsfc</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr"/>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="C11" t="inlineStr">
         <is>
           <t>SurfaceInitialState (state.py, 15)</t>
@@ -714,7 +746,11 @@
           <t>bsoil.icefrac</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr"/>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C12" t="inlineStr">
         <is>
           <t>SurfaceInitialState (state.py, 15)</t>
@@ -738,7 +774,11 @@
           <t>bsoil.snowdens</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr"/>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C13" t="inlineStr">
         <is>
           <t>SurfaceInitialState (state.py, 15)</t>
@@ -762,7 +802,11 @@
           <t>bsoil.snowfrac</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr"/>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C14" t="inlineStr">
         <is>
           <t>SurfaceInitialState (state.py, 15)</t>
@@ -786,7 +830,11 @@
           <t>bsoil.snowpack</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr"/>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C15" t="inlineStr">
         <is>
           <t>SurfaceInitialState (state.py, 15)</t>
@@ -810,7 +858,11 @@
           <t>bsoil.snowwater</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr"/>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C16" t="inlineStr">
         <is>
           <t>SurfaceInitialState (state.py, 15)</t>
@@ -882,7 +934,11 @@
           <t>bsoil.temperature</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr"/>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="C19" t="inlineStr">
         <is>
           <t>RefValue (type.py, 33); SurfaceInitialState (state.py, 15); validate_temperature (state.py, 82)</t>
@@ -906,7 +962,11 @@
           <t>bsoil.tin</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr"/>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="C20" t="inlineStr">
         <is>
           <t>SurfaceInitialState (state.py, 15)</t>
@@ -930,7 +990,11 @@
           <t>bsoil.tsfc</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr"/>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="C21" t="inlineStr">
         <is>
           <t>SurfaceInitialState (state.py, 15)</t>
@@ -1026,7 +1090,11 @@
           <t>dectr.icefrac</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr"/>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C25" t="inlineStr">
         <is>
           <t>SurfaceInitialState (state.py, 15)</t>
@@ -1122,7 +1190,11 @@
           <t>dectr.snowdens</t>
         </is>
       </c>
-      <c r="B29" t="inlineStr"/>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C29" t="inlineStr">
         <is>
           <t>SurfaceInitialState (state.py, 15)</t>
@@ -1146,7 +1218,11 @@
           <t>dectr.snowfrac</t>
         </is>
       </c>
-      <c r="B30" t="inlineStr"/>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C30" t="inlineStr">
         <is>
           <t>SurfaceInitialState (state.py, 15)</t>
@@ -1170,7 +1246,11 @@
           <t>dectr.snowpack</t>
         </is>
       </c>
-      <c r="B31" t="inlineStr"/>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C31" t="inlineStr">
         <is>
           <t>SurfaceInitialState (state.py, 15)</t>
@@ -1194,7 +1274,11 @@
           <t>dectr.snowwater</t>
         </is>
       </c>
-      <c r="B32" t="inlineStr"/>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C32" t="inlineStr">
         <is>
           <t>SurfaceInitialState (state.py, 15)</t>
@@ -1266,7 +1350,11 @@
           <t>dectr.temperature</t>
         </is>
       </c>
-      <c r="B35" t="inlineStr"/>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="C35" t="inlineStr">
         <is>
           <t>RefValue (type.py, 33); SurfaceInitialState (state.py, 15); validate_temperature (state.py, 82)</t>
@@ -1290,7 +1378,11 @@
           <t>dectr.tin</t>
         </is>
       </c>
-      <c r="B36" t="inlineStr"/>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="C36" t="inlineStr">
         <is>
           <t>SurfaceInitialState (state.py, 15)</t>
@@ -1314,7 +1406,11 @@
           <t>dectr.tsfc</t>
         </is>
       </c>
-      <c r="B37" t="inlineStr"/>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="C37" t="inlineStr">
         <is>
           <t>SurfaceInitialState (state.py, 15)</t>
@@ -1530,7 +1626,11 @@
           <t>evetr.icefrac</t>
         </is>
       </c>
-      <c r="B46" t="inlineStr"/>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C46" t="inlineStr">
         <is>
           <t>SurfaceInitialState (state.py, 15)</t>
@@ -1602,7 +1702,11 @@
           <t>evetr.snowdens</t>
         </is>
       </c>
-      <c r="B49" t="inlineStr"/>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C49" t="inlineStr">
         <is>
           <t>SurfaceInitialState (state.py, 15)</t>
@@ -1626,7 +1730,11 @@
           <t>evetr.snowfrac</t>
         </is>
       </c>
-      <c r="B50" t="inlineStr"/>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C50" t="inlineStr">
         <is>
           <t>SurfaceInitialState (state.py, 15)</t>
@@ -1650,7 +1758,11 @@
           <t>evetr.snowpack</t>
         </is>
       </c>
-      <c r="B51" t="inlineStr"/>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C51" t="inlineStr">
         <is>
           <t>SurfaceInitialState (state.py, 15)</t>
@@ -1674,7 +1786,11 @@
           <t>evetr.snowwater</t>
         </is>
       </c>
-      <c r="B52" t="inlineStr"/>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C52" t="inlineStr">
         <is>
           <t>SurfaceInitialState (state.py, 15)</t>
@@ -1746,7 +1862,11 @@
           <t>evetr.temperature</t>
         </is>
       </c>
-      <c r="B55" t="inlineStr"/>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="C55" t="inlineStr">
         <is>
           <t>RefValue (type.py, 33); SurfaceInitialState (state.py, 15); validate_temperature (state.py, 82)</t>
@@ -1770,7 +1890,11 @@
           <t>evetr.tin</t>
         </is>
       </c>
-      <c r="B56" t="inlineStr"/>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="C56" t="inlineStr">
         <is>
           <t>SurfaceInitialState (state.py, 15)</t>
@@ -1794,7 +1918,11 @@
           <t>evetr.tsfc</t>
         </is>
       </c>
-      <c r="B57" t="inlineStr"/>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="C57" t="inlineStr">
         <is>
           <t>SurfaceInitialState (state.py, 15)</t>
@@ -1938,7 +2066,11 @@
           <t>grass.icefrac</t>
         </is>
       </c>
-      <c r="B63" t="inlineStr"/>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C63" t="inlineStr">
         <is>
           <t>SurfaceInitialState (state.py, 15)</t>
@@ -2010,7 +2142,11 @@
           <t>grass.snowdens</t>
         </is>
       </c>
-      <c r="B66" t="inlineStr"/>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C66" t="inlineStr">
         <is>
           <t>SurfaceInitialState (state.py, 15)</t>
@@ -2034,7 +2170,11 @@
           <t>grass.snowfrac</t>
         </is>
       </c>
-      <c r="B67" t="inlineStr"/>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C67" t="inlineStr">
         <is>
           <t>SurfaceInitialState (state.py, 15)</t>
@@ -2058,7 +2198,11 @@
           <t>grass.snowpack</t>
         </is>
       </c>
-      <c r="B68" t="inlineStr"/>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C68" t="inlineStr">
         <is>
           <t>SurfaceInitialState (state.py, 15)</t>
@@ -2082,7 +2226,11 @@
           <t>grass.snowwater</t>
         </is>
       </c>
-      <c r="B69" t="inlineStr"/>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C69" t="inlineStr">
         <is>
           <t>SurfaceInitialState (state.py, 15)</t>
@@ -2154,7 +2302,11 @@
           <t>grass.temperature</t>
         </is>
       </c>
-      <c r="B72" t="inlineStr"/>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="C72" t="inlineStr">
         <is>
           <t>RefValue (type.py, 33); SurfaceInitialState (state.py, 15); validate_temperature (state.py, 82)</t>
@@ -2178,7 +2330,11 @@
           <t>grass.tin</t>
         </is>
       </c>
-      <c r="B73" t="inlineStr"/>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="C73" t="inlineStr">
         <is>
           <t>SurfaceInitialState (state.py, 15)</t>
@@ -2202,7 +2358,11 @@
           <t>grass.tsfc</t>
         </is>
       </c>
-      <c r="B74" t="inlineStr"/>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="C74" t="inlineStr">
         <is>
           <t>SurfaceInitialState (state.py, 15)</t>
@@ -2346,7 +2506,11 @@
           <t>paved.icefrac</t>
         </is>
       </c>
-      <c r="B80" t="inlineStr"/>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C80" t="inlineStr">
         <is>
           <t>SurfaceInitialState (state.py, 15)</t>
@@ -2370,7 +2534,11 @@
           <t>paved.snowdens</t>
         </is>
       </c>
-      <c r="B81" t="inlineStr"/>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C81" t="inlineStr">
         <is>
           <t>SurfaceInitialState (state.py, 15)</t>
@@ -2394,7 +2562,11 @@
           <t>paved.snowfrac</t>
         </is>
       </c>
-      <c r="B82" t="inlineStr"/>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C82" t="inlineStr">
         <is>
           <t>SurfaceInitialState (state.py, 15)</t>
@@ -2418,7 +2590,11 @@
           <t>paved.snowpack</t>
         </is>
       </c>
-      <c r="B83" t="inlineStr"/>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C83" t="inlineStr">
         <is>
           <t>SurfaceInitialState (state.py, 15)</t>
@@ -2442,7 +2618,11 @@
           <t>paved.snowwater</t>
         </is>
       </c>
-      <c r="B84" t="inlineStr"/>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C84" t="inlineStr">
         <is>
           <t>SurfaceInitialState (state.py, 15)</t>
@@ -2514,7 +2694,11 @@
           <t>paved.temperature</t>
         </is>
       </c>
-      <c r="B87" t="inlineStr"/>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="C87" t="inlineStr">
         <is>
           <t>RefValue (type.py, 33); SurfaceInitialState (state.py, 15); validate_temperature (state.py, 82)</t>
@@ -2538,7 +2722,11 @@
           <t>paved.tin</t>
         </is>
       </c>
-      <c r="B88" t="inlineStr"/>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="C88" t="inlineStr">
         <is>
           <t>SurfaceInitialState (state.py, 15)</t>
@@ -2562,7 +2750,11 @@
           <t>paved.tsfc</t>
         </is>
       </c>
-      <c r="B89" t="inlineStr"/>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="C89" t="inlineStr">
         <is>
           <t>SurfaceInitialState (state.py, 15)</t>
@@ -2658,7 +2850,11 @@
           <t>snowalb</t>
         </is>
       </c>
-      <c r="B93" t="inlineStr"/>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C93" t="inlineStr">
         <is>
           <t>validate_snow_parameters (core.py, 372); SnowAlb (site.py, 2481); InitialStates (state.py, 761)</t>
@@ -2682,7 +2878,11 @@
           <t>snowfallcum</t>
         </is>
       </c>
-      <c r="B94" t="inlineStr"/>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C94" t="inlineStr">
         <is>
           <t>InitialStates (state.py, 761)</t>
@@ -2826,7 +3026,11 @@
           <t>water.icefrac</t>
         </is>
       </c>
-      <c r="B100" t="inlineStr"/>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C100" t="inlineStr">
         <is>
           <t>SurfaceInitialState (state.py, 15)</t>
@@ -2850,7 +3054,11 @@
           <t>water.snowdens</t>
         </is>
       </c>
-      <c r="B101" t="inlineStr"/>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C101" t="inlineStr">
         <is>
           <t>SurfaceInitialState (state.py, 15)</t>
@@ -2874,7 +3082,11 @@
           <t>water.snowfrac</t>
         </is>
       </c>
-      <c r="B102" t="inlineStr"/>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C102" t="inlineStr">
         <is>
           <t>SurfaceInitialState (state.py, 15)</t>
@@ -2898,7 +3110,11 @@
           <t>water.snowpack</t>
         </is>
       </c>
-      <c r="B103" t="inlineStr"/>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C103" t="inlineStr">
         <is>
           <t>SurfaceInitialState (state.py, 15)</t>
@@ -2922,7 +3138,11 @@
           <t>water.snowwater</t>
         </is>
       </c>
-      <c r="B104" t="inlineStr"/>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C104" t="inlineStr">
         <is>
           <t>SurfaceInitialState (state.py, 15)</t>
@@ -2994,7 +3214,11 @@
           <t>water.temperature</t>
         </is>
       </c>
-      <c r="B107" t="inlineStr"/>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="C107" t="inlineStr">
         <is>
           <t>RefValue (type.py, 33); SurfaceInitialState (state.py, 15); validate_temperature (state.py, 82)</t>
@@ -3018,7 +3242,11 @@
           <t>water.tin</t>
         </is>
       </c>
-      <c r="B108" t="inlineStr"/>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="C108" t="inlineStr">
         <is>
           <t>SurfaceInitialState (state.py, 15)</t>
@@ -3042,7 +3270,11 @@
           <t>water.tsfc</t>
         </is>
       </c>
-      <c r="B109" t="inlineStr"/>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="C109" t="inlineStr">
         <is>
           <t>SurfaceInitialState (state.py, 15)</t>
@@ -13584,7 +13816,11 @@
           <t>land_cover.bldgs.snowpacklimit</t>
         </is>
       </c>
-      <c r="B425" t="inlineStr"/>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C425" t="inlineStr">
         <is>
           <t>SurfaceProperties (surface.py, 159)</t>
@@ -14616,7 +14852,11 @@
           <t>land_cover.bsoil.snowpacklimit</t>
         </is>
       </c>
-      <c r="B468" t="inlineStr"/>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C468" t="inlineStr">
         <is>
           <t>SurfaceProperties (surface.py, 159)</t>
@@ -16344,7 +16584,11 @@
           <t>land_cover.dectr.snowpacklimit</t>
         </is>
       </c>
-      <c r="B540" t="inlineStr"/>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C540" t="inlineStr">
         <is>
           <t>SurfaceProperties (surface.py, 159)</t>
@@ -18000,7 +18244,11 @@
           <t>land_cover.evetr.snowpacklimit</t>
         </is>
       </c>
-      <c r="B609" t="inlineStr"/>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C609" t="inlineStr">
         <is>
           <t>SurfaceProperties (surface.py, 159)</t>
@@ -19608,7 +19856,11 @@
           <t>land_cover.grass.snowpacklimit</t>
         </is>
       </c>
-      <c r="B676" t="inlineStr"/>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C676" t="inlineStr">
         <is>
           <t>SurfaceProperties (surface.py, 159)</t>
@@ -20664,7 +20916,11 @@
           <t>land_cover.paved.snowpacklimit</t>
         </is>
       </c>
-      <c r="B720" t="inlineStr"/>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C720" t="inlineStr">
         <is>
           <t>SurfaceProperties (surface.py, 159)</t>
@@ -21720,7 +21976,11 @@
           <t>land_cover.water.snowpacklimit</t>
         </is>
       </c>
-      <c r="B764" t="inlineStr"/>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C764" t="inlineStr">
         <is>
           <t>SurfaceProperties (surface.py, 159)</t>
@@ -22296,7 +22556,11 @@
           <t>snow.crwmax</t>
         </is>
       </c>
-      <c r="B788" t="inlineStr"/>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C788" t="inlineStr">
         <is>
           <t>validate_snow_parameters (core.py, 372); SnowParams (site.py, 842)</t>
@@ -22320,7 +22584,11 @@
           <t>snow.crwmin</t>
         </is>
       </c>
-      <c r="B789" t="inlineStr"/>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C789" t="inlineStr">
         <is>
           <t>validate_snow_parameters (core.py, 372); SnowParams (site.py, 842)</t>
@@ -22344,7 +22612,11 @@
           <t>snow.narp_emis_snow</t>
         </is>
       </c>
-      <c r="B790" t="inlineStr"/>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C790" t="inlineStr">
         <is>
           <t>SnowParams (site.py, 842)</t>
@@ -22368,7 +22640,11 @@
           <t>snow.preciplimit</t>
         </is>
       </c>
-      <c r="B791" t="inlineStr"/>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C791" t="inlineStr">
         <is>
           <t>SnowParams (site.py, 842)</t>
@@ -22392,7 +22668,11 @@
           <t>snow.preciplimitalb</t>
         </is>
       </c>
-      <c r="B792" t="inlineStr"/>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C792" t="inlineStr">
         <is>
           <t>SnowParams (site.py, 842)</t>
@@ -22416,7 +22696,11 @@
           <t>snow.radmeltfact</t>
         </is>
       </c>
-      <c r="B793" t="inlineStr"/>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C793" t="inlineStr">
         <is>
           <t>SnowParams (site.py, 842)</t>
@@ -22440,7 +22724,11 @@
           <t>snow.snowalbmax</t>
         </is>
       </c>
-      <c r="B794" t="inlineStr"/>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C794" t="inlineStr">
         <is>
           <t>validate_snow_parameters (core.py, 372); SnowParams (site.py, 842)</t>
@@ -22464,7 +22752,11 @@
           <t>snow.snowalbmin</t>
         </is>
       </c>
-      <c r="B795" t="inlineStr"/>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C795" t="inlineStr">
         <is>
           <t>validate_snow_parameters (core.py, 372); SnowParams (site.py, 842)</t>
@@ -22488,7 +22780,11 @@
           <t>snow.snowdensmax</t>
         </is>
       </c>
-      <c r="B796" t="inlineStr"/>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C796" t="inlineStr">
         <is>
           <t>SnowParams (site.py, 842)</t>
@@ -22512,7 +22808,11 @@
           <t>snow.snowdensmin</t>
         </is>
       </c>
-      <c r="B797" t="inlineStr"/>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C797" t="inlineStr">
         <is>
           <t>SnowParams (site.py, 842)</t>
@@ -22536,7 +22836,11 @@
           <t>snow.snowlimbldg</t>
         </is>
       </c>
-      <c r="B798" t="inlineStr"/>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C798" t="inlineStr">
         <is>
           <t>SnowParams (site.py, 842)</t>
@@ -22560,7 +22864,11 @@
           <t>snow.snowlimpaved</t>
         </is>
       </c>
-      <c r="B799" t="inlineStr"/>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C799" t="inlineStr">
         <is>
           <t>SnowParams (site.py, 842)</t>
@@ -22584,7 +22892,11 @@
           <t>snow.snowprof_24hr.holiday.1</t>
         </is>
       </c>
-      <c r="B800" t="inlineStr"/>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C800" t="inlineStr">
         <is>
           <t>No Pydantic usage found</t>
@@ -22608,7 +22920,11 @@
           <t>snow.snowprof_24hr.holiday.10</t>
         </is>
       </c>
-      <c r="B801" t="inlineStr"/>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C801" t="inlineStr">
         <is>
           <t>No Pydantic usage found</t>
@@ -22632,7 +22948,11 @@
           <t>snow.snowprof_24hr.holiday.11</t>
         </is>
       </c>
-      <c r="B802" t="inlineStr"/>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C802" t="inlineStr">
         <is>
           <t>No Pydantic usage found</t>
@@ -22656,7 +22976,11 @@
           <t>snow.snowprof_24hr.holiday.12</t>
         </is>
       </c>
-      <c r="B803" t="inlineStr"/>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C803" t="inlineStr">
         <is>
           <t>No Pydantic usage found</t>
@@ -22680,7 +23004,11 @@
           <t>snow.snowprof_24hr.holiday.13</t>
         </is>
       </c>
-      <c r="B804" t="inlineStr"/>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C804" t="inlineStr">
         <is>
           <t>No Pydantic usage found</t>
@@ -22704,7 +23032,11 @@
           <t>snow.snowprof_24hr.holiday.14</t>
         </is>
       </c>
-      <c r="B805" t="inlineStr"/>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C805" t="inlineStr">
         <is>
           <t>No Pydantic usage found</t>
@@ -22728,7 +23060,11 @@
           <t>snow.snowprof_24hr.holiday.15</t>
         </is>
       </c>
-      <c r="B806" t="inlineStr"/>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C806" t="inlineStr">
         <is>
           <t>No Pydantic usage found</t>
@@ -22752,7 +23088,11 @@
           <t>snow.snowprof_24hr.holiday.16</t>
         </is>
       </c>
-      <c r="B807" t="inlineStr"/>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C807" t="inlineStr">
         <is>
           <t>No Pydantic usage found</t>
@@ -22776,7 +23116,11 @@
           <t>snow.snowprof_24hr.holiday.17</t>
         </is>
       </c>
-      <c r="B808" t="inlineStr"/>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C808" t="inlineStr">
         <is>
           <t>No Pydantic usage found</t>
@@ -22800,7 +23144,11 @@
           <t>snow.snowprof_24hr.holiday.18</t>
         </is>
       </c>
-      <c r="B809" t="inlineStr"/>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C809" t="inlineStr">
         <is>
           <t>No Pydantic usage found</t>
@@ -22824,7 +23172,11 @@
           <t>snow.snowprof_24hr.holiday.19</t>
         </is>
       </c>
-      <c r="B810" t="inlineStr"/>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C810" t="inlineStr">
         <is>
           <t>No Pydantic usage found</t>
@@ -22848,7 +23200,11 @@
           <t>snow.snowprof_24hr.holiday.2</t>
         </is>
       </c>
-      <c r="B811" t="inlineStr"/>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C811" t="inlineStr">
         <is>
           <t>No Pydantic usage found</t>
@@ -22872,7 +23228,11 @@
           <t>snow.snowprof_24hr.holiday.20</t>
         </is>
       </c>
-      <c r="B812" t="inlineStr"/>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C812" t="inlineStr">
         <is>
           <t>No Pydantic usage found</t>
@@ -22896,7 +23256,11 @@
           <t>snow.snowprof_24hr.holiday.21</t>
         </is>
       </c>
-      <c r="B813" t="inlineStr"/>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C813" t="inlineStr">
         <is>
           <t>No Pydantic usage found</t>
@@ -22920,7 +23284,11 @@
           <t>snow.snowprof_24hr.holiday.22</t>
         </is>
       </c>
-      <c r="B814" t="inlineStr"/>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C814" t="inlineStr">
         <is>
           <t>No Pydantic usage found</t>
@@ -22944,7 +23312,11 @@
           <t>snow.snowprof_24hr.holiday.23</t>
         </is>
       </c>
-      <c r="B815" t="inlineStr"/>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C815" t="inlineStr">
         <is>
           <t>No Pydantic usage found</t>
@@ -22968,7 +23340,11 @@
           <t>snow.snowprof_24hr.holiday.24</t>
         </is>
       </c>
-      <c r="B816" t="inlineStr"/>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C816" t="inlineStr">
         <is>
           <t>No Pydantic usage found</t>
@@ -22992,7 +23368,11 @@
           <t>snow.snowprof_24hr.holiday.3</t>
         </is>
       </c>
-      <c r="B817" t="inlineStr"/>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C817" t="inlineStr">
         <is>
           <t>No Pydantic usage found</t>
@@ -23016,7 +23396,11 @@
           <t>snow.snowprof_24hr.holiday.4</t>
         </is>
       </c>
-      <c r="B818" t="inlineStr"/>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C818" t="inlineStr">
         <is>
           <t>No Pydantic usage found</t>
@@ -23040,7 +23424,11 @@
           <t>snow.snowprof_24hr.holiday.5</t>
         </is>
       </c>
-      <c r="B819" t="inlineStr"/>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C819" t="inlineStr">
         <is>
           <t>No Pydantic usage found</t>
@@ -23064,7 +23452,11 @@
           <t>snow.snowprof_24hr.holiday.6</t>
         </is>
       </c>
-      <c r="B820" t="inlineStr"/>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C820" t="inlineStr">
         <is>
           <t>No Pydantic usage found</t>
@@ -23088,7 +23480,11 @@
           <t>snow.snowprof_24hr.holiday.7</t>
         </is>
       </c>
-      <c r="B821" t="inlineStr"/>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C821" t="inlineStr">
         <is>
           <t>No Pydantic usage found</t>
@@ -23112,7 +23508,11 @@
           <t>snow.snowprof_24hr.holiday.8</t>
         </is>
       </c>
-      <c r="B822" t="inlineStr"/>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C822" t="inlineStr">
         <is>
           <t>No Pydantic usage found</t>
@@ -23136,7 +23536,11 @@
           <t>snow.snowprof_24hr.holiday.9</t>
         </is>
       </c>
-      <c r="B823" t="inlineStr"/>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C823" t="inlineStr">
         <is>
           <t>No Pydantic usage found</t>
@@ -23160,7 +23564,11 @@
           <t>snow.snowprof_24hr.working_day.1</t>
         </is>
       </c>
-      <c r="B824" t="inlineStr"/>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C824" t="inlineStr">
         <is>
           <t>No Pydantic usage found</t>
@@ -23184,7 +23592,11 @@
           <t>snow.snowprof_24hr.working_day.10</t>
         </is>
       </c>
-      <c r="B825" t="inlineStr"/>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C825" t="inlineStr">
         <is>
           <t>No Pydantic usage found</t>
@@ -23208,7 +23620,11 @@
           <t>snow.snowprof_24hr.working_day.11</t>
         </is>
       </c>
-      <c r="B826" t="inlineStr"/>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C826" t="inlineStr">
         <is>
           <t>No Pydantic usage found</t>
@@ -23232,7 +23648,11 @@
           <t>snow.snowprof_24hr.working_day.12</t>
         </is>
       </c>
-      <c r="B827" t="inlineStr"/>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C827" t="inlineStr">
         <is>
           <t>No Pydantic usage found</t>
@@ -23256,7 +23676,11 @@
           <t>snow.snowprof_24hr.working_day.13</t>
         </is>
       </c>
-      <c r="B828" t="inlineStr"/>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C828" t="inlineStr">
         <is>
           <t>No Pydantic usage found</t>
@@ -23280,7 +23704,11 @@
           <t>snow.snowprof_24hr.working_day.14</t>
         </is>
       </c>
-      <c r="B829" t="inlineStr"/>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C829" t="inlineStr">
         <is>
           <t>No Pydantic usage found</t>
@@ -23304,7 +23732,11 @@
           <t>snow.snowprof_24hr.working_day.15</t>
         </is>
       </c>
-      <c r="B830" t="inlineStr"/>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C830" t="inlineStr">
         <is>
           <t>No Pydantic usage found</t>
@@ -23328,7 +23760,11 @@
           <t>snow.snowprof_24hr.working_day.16</t>
         </is>
       </c>
-      <c r="B831" t="inlineStr"/>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C831" t="inlineStr">
         <is>
           <t>No Pydantic usage found</t>
@@ -23352,7 +23788,11 @@
           <t>snow.snowprof_24hr.working_day.17</t>
         </is>
       </c>
-      <c r="B832" t="inlineStr"/>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C832" t="inlineStr">
         <is>
           <t>No Pydantic usage found</t>
@@ -23376,7 +23816,11 @@
           <t>snow.snowprof_24hr.working_day.18</t>
         </is>
       </c>
-      <c r="B833" t="inlineStr"/>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C833" t="inlineStr">
         <is>
           <t>No Pydantic usage found</t>
@@ -23400,7 +23844,11 @@
           <t>snow.snowprof_24hr.working_day.19</t>
         </is>
       </c>
-      <c r="B834" t="inlineStr"/>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C834" t="inlineStr">
         <is>
           <t>No Pydantic usage found</t>
@@ -23424,7 +23872,11 @@
           <t>snow.snowprof_24hr.working_day.2</t>
         </is>
       </c>
-      <c r="B835" t="inlineStr"/>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C835" t="inlineStr">
         <is>
           <t>No Pydantic usage found</t>
@@ -23448,7 +23900,11 @@
           <t>snow.snowprof_24hr.working_day.20</t>
         </is>
       </c>
-      <c r="B836" t="inlineStr"/>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C836" t="inlineStr">
         <is>
           <t>No Pydantic usage found</t>
@@ -23472,7 +23928,11 @@
           <t>snow.snowprof_24hr.working_day.21</t>
         </is>
       </c>
-      <c r="B837" t="inlineStr"/>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C837" t="inlineStr">
         <is>
           <t>No Pydantic usage found</t>
@@ -23496,7 +23956,11 @@
           <t>snow.snowprof_24hr.working_day.22</t>
         </is>
       </c>
-      <c r="B838" t="inlineStr"/>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C838" t="inlineStr">
         <is>
           <t>No Pydantic usage found</t>
@@ -23520,7 +23984,11 @@
           <t>snow.snowprof_24hr.working_day.23</t>
         </is>
       </c>
-      <c r="B839" t="inlineStr"/>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C839" t="inlineStr">
         <is>
           <t>No Pydantic usage found</t>
@@ -23544,7 +24012,11 @@
           <t>snow.snowprof_24hr.working_day.24</t>
         </is>
       </c>
-      <c r="B840" t="inlineStr"/>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C840" t="inlineStr">
         <is>
           <t>No Pydantic usage found</t>
@@ -23568,7 +24040,11 @@
           <t>snow.snowprof_24hr.working_day.3</t>
         </is>
       </c>
-      <c r="B841" t="inlineStr"/>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C841" t="inlineStr">
         <is>
           <t>No Pydantic usage found</t>
@@ -23592,7 +24068,11 @@
           <t>snow.snowprof_24hr.working_day.4</t>
         </is>
       </c>
-      <c r="B842" t="inlineStr"/>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C842" t="inlineStr">
         <is>
           <t>No Pydantic usage found</t>
@@ -23616,7 +24096,11 @@
           <t>snow.snowprof_24hr.working_day.5</t>
         </is>
       </c>
-      <c r="B843" t="inlineStr"/>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C843" t="inlineStr">
         <is>
           <t>No Pydantic usage found</t>
@@ -23640,7 +24124,11 @@
           <t>snow.snowprof_24hr.working_day.6</t>
         </is>
       </c>
-      <c r="B844" t="inlineStr"/>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C844" t="inlineStr">
         <is>
           <t>No Pydantic usage found</t>
@@ -23664,7 +24152,11 @@
           <t>snow.snowprof_24hr.working_day.7</t>
         </is>
       </c>
-      <c r="B845" t="inlineStr"/>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C845" t="inlineStr">
         <is>
           <t>No Pydantic usage found</t>
@@ -23688,7 +24180,11 @@
           <t>snow.snowprof_24hr.working_day.8</t>
         </is>
       </c>
-      <c r="B846" t="inlineStr"/>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C846" t="inlineStr">
         <is>
           <t>No Pydantic usage found</t>
@@ -23712,7 +24208,11 @@
           <t>snow.snowprof_24hr.working_day.9</t>
         </is>
       </c>
-      <c r="B847" t="inlineStr"/>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C847" t="inlineStr">
         <is>
           <t>No Pydantic usage found</t>
@@ -23736,7 +24236,11 @@
           <t>snow.tau_a</t>
         </is>
       </c>
-      <c r="B848" t="inlineStr"/>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C848" t="inlineStr">
         <is>
           <t>SnowParams (site.py, 842)</t>
@@ -23760,7 +24264,11 @@
           <t>snow.tau_f</t>
         </is>
       </c>
-      <c r="B849" t="inlineStr"/>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C849" t="inlineStr">
         <is>
           <t>SnowParams (site.py, 842)</t>
@@ -23784,7 +24292,11 @@
           <t>snow.tau_r</t>
         </is>
       </c>
-      <c r="B850" t="inlineStr"/>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C850" t="inlineStr">
         <is>
           <t>SnowParams (site.py, 842)</t>
@@ -23808,7 +24320,11 @@
           <t>snow.tempmeltfact</t>
         </is>
       </c>
-      <c r="B851" t="inlineStr"/>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="C851" t="inlineStr">
         <is>
           <t>SnowParams (site.py, 842)</t>

</xml_diff>

<commit_message>
add: note 4 and 10
Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/src/supy/data_model/initial_states/parameter_analysis.xlsx
+++ b/src/supy/data_model/initial_states/parameter_analysis.xlsx
@@ -614,7 +614,11 @@
           <t>bldgs.soilstore</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr"/>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
       <c r="C7" t="inlineStr">
         <is>
           <t>WaterDistribution (hydro.py, 8); SurfaceInitialState (state.py, 15)</t>
@@ -638,7 +642,11 @@
           <t>bldgs.state</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr"/>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
       <c r="C8" t="inlineStr">
         <is>
           <t>No Pydantic usage found</t>
@@ -886,7 +894,11 @@
           <t>bsoil.soilstore</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr"/>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
       <c r="C17" t="inlineStr">
         <is>
           <t>WaterDistribution (hydro.py, 8); SurfaceInitialState (state.py, 15)</t>
@@ -910,7 +922,11 @@
           <t>bsoil.state</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr"/>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
       <c r="C18" t="inlineStr">
         <is>
           <t>No Pydantic usage found</t>
@@ -1066,7 +1082,11 @@
           <t>dectr.gdd_id</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr"/>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
       <c r="C24" t="inlineStr">
         <is>
           <t>VegetationParams (site.py, 37); InitialStateVeg (state.py, 321)</t>
@@ -1166,7 +1186,11 @@
           <t>dectr.sdd_id</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr"/>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
       <c r="C28" t="inlineStr">
         <is>
           <t>VegetationParams (site.py, 37); InitialStateVeg (state.py, 321)</t>
@@ -1302,7 +1326,11 @@
           <t>dectr.soilstore</t>
         </is>
       </c>
-      <c r="B33" t="inlineStr"/>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
       <c r="C33" t="inlineStr">
         <is>
           <t>WaterDistribution (hydro.py, 8); SurfaceInitialState (state.py, 15)</t>
@@ -1326,7 +1354,11 @@
           <t>dectr.state</t>
         </is>
       </c>
-      <c r="B34" t="inlineStr"/>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
       <c r="C34" t="inlineStr">
         <is>
           <t>No Pydantic usage found</t>
@@ -1602,7 +1634,11 @@
           <t>evetr.gdd_id</t>
         </is>
       </c>
-      <c r="B45" t="inlineStr"/>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
       <c r="C45" t="inlineStr">
         <is>
           <t>VegetationParams (site.py, 37); InitialStateVeg (state.py, 321)</t>
@@ -1678,7 +1714,11 @@
           <t>evetr.sdd_id</t>
         </is>
       </c>
-      <c r="B48" t="inlineStr"/>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
       <c r="C48" t="inlineStr">
         <is>
           <t>VegetationParams (site.py, 37); InitialStateVeg (state.py, 321)</t>
@@ -1814,7 +1854,11 @@
           <t>evetr.soilstore</t>
         </is>
       </c>
-      <c r="B53" t="inlineStr"/>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
       <c r="C53" t="inlineStr">
         <is>
           <t>WaterDistribution (hydro.py, 8); SurfaceInitialState (state.py, 15)</t>
@@ -1838,7 +1882,11 @@
           <t>evetr.state</t>
         </is>
       </c>
-      <c r="B54" t="inlineStr"/>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
       <c r="C54" t="inlineStr">
         <is>
           <t>No Pydantic usage found</t>
@@ -2042,7 +2090,11 @@
           <t>grass.gdd_id</t>
         </is>
       </c>
-      <c r="B62" t="inlineStr"/>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
       <c r="C62" t="inlineStr">
         <is>
           <t>VegetationParams (site.py, 37); InitialStateVeg (state.py, 321)</t>
@@ -2118,7 +2170,11 @@
           <t>grass.sdd_id</t>
         </is>
       </c>
-      <c r="B65" t="inlineStr"/>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
       <c r="C65" t="inlineStr">
         <is>
           <t>VegetationParams (site.py, 37); InitialStateVeg (state.py, 321)</t>
@@ -2254,7 +2310,11 @@
           <t>grass.soilstore</t>
         </is>
       </c>
-      <c r="B70" t="inlineStr"/>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
       <c r="C70" t="inlineStr">
         <is>
           <t>WaterDistribution (hydro.py, 8); SurfaceInitialState (state.py, 15)</t>
@@ -2278,7 +2338,11 @@
           <t>grass.state</t>
         </is>
       </c>
-      <c r="B71" t="inlineStr"/>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
       <c r="C71" t="inlineStr">
         <is>
           <t>No Pydantic usage found</t>
@@ -2458,7 +2522,11 @@
           <t>hdd_id</t>
         </is>
       </c>
-      <c r="B78" t="inlineStr"/>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
       <c r="C78" t="inlineStr">
         <is>
           <t>InitialStates (state.py, 761)</t>
@@ -2646,7 +2714,11 @@
           <t>paved.soilstore</t>
         </is>
       </c>
-      <c r="B85" t="inlineStr"/>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
       <c r="C85" t="inlineStr">
         <is>
           <t>WaterDistribution (hydro.py, 8); SurfaceInitialState (state.py, 15)</t>
@@ -2670,7 +2742,11 @@
           <t>paved.state</t>
         </is>
       </c>
-      <c r="B86" t="inlineStr"/>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
       <c r="C86" t="inlineStr">
         <is>
           <t>No Pydantic usage found</t>
@@ -2829,7 +2905,7 @@
       <c r="B92" t="inlineStr"/>
       <c r="C92" t="inlineStr">
         <is>
-          <t>SUEWSConfig (core.py, 94); validate_building_layers (core.py, 1533); VerticalLayers (surface.py, 976); InitialStates (state.py, 761)</t>
+          <t>SUEWSConfig (core.py, 94); validate_building_layers (core.py, 1569); VerticalLayers (surface.py, 976); InitialStates (state.py, 761)</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
@@ -2906,7 +2982,11 @@
           <t>tair_av</t>
         </is>
       </c>
-      <c r="B95" t="inlineStr"/>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="C95" t="inlineStr">
         <is>
           <t>InitialStates (state.py, 761)</t>
@@ -2930,7 +3010,11 @@
           <t>tmax_id</t>
         </is>
       </c>
-      <c r="B96" t="inlineStr"/>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="C96" t="inlineStr">
         <is>
           <t>InitialStates (state.py, 761)</t>
@@ -2954,7 +3038,11 @@
           <t>tmin_id</t>
         </is>
       </c>
-      <c r="B97" t="inlineStr"/>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="C97" t="inlineStr">
         <is>
           <t>InitialStates (state.py, 761)</t>
@@ -3005,7 +3093,7 @@
       <c r="B99" t="inlineStr"/>
       <c r="C99" t="inlineStr">
         <is>
-          <t>SUEWSConfig (core.py, 94); _validate_storage (core.py, 1144); validate_building_layers (core.py, 1533); VerticalLayers (surface.py, 976); InitialStates (state.py, 761)</t>
+          <t>SUEWSConfig (core.py, 94); _validate_storage (core.py, 1166); validate_building_layers (core.py, 1569); VerticalLayers (surface.py, 976); InitialStates (state.py, 761)</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
@@ -3166,7 +3254,11 @@
           <t>water.soilstore</t>
         </is>
       </c>
-      <c r="B105" t="inlineStr"/>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
       <c r="C105" t="inlineStr">
         <is>
           <t>WaterDistribution (hydro.py, 8); SurfaceInitialState (state.py, 15)</t>
@@ -3190,7 +3282,11 @@
           <t>water.state</t>
         </is>
       </c>
-      <c r="B106" t="inlineStr"/>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
       <c r="C106" t="inlineStr">
         <is>
           <t>No Pydantic usage found</t>
@@ -3691,7 +3787,7 @@
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr">
         <is>
-          <t>SUEWSConfig (core.py, 94); _check_co2_params (core.py, 672); CO2Params (human_activity.py, 339); YAMLAnnotator (yaml_annotator.py, 32); ValidationIssue (yaml_annotator_json.py, 16)</t>
+          <t>SUEWSConfig (core.py, 94); _check_co2_params (core.py, 694); CO2Params (human_activity.py, 339); YAMLAnnotator (yaml_annotator.py, 32); ValidationIssue (yaml_annotator_json.py, 16)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -3715,7 +3811,7 @@
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr">
         <is>
-          <t>SUEWSConfig (core.py, 94); _check_co2_params (core.py, 672); CO2Params (human_activity.py, 339); YAMLAnnotator (yaml_annotator.py, 32); ValidationIssue (yaml_annotator_json.py, 16)</t>
+          <t>SUEWSConfig (core.py, 94); _check_co2_params (core.py, 694); CO2Params (human_activity.py, 339); YAMLAnnotator (yaml_annotator.py, 32); ValidationIssue (yaml_annotator_json.py, 16)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -3763,7 +3859,7 @@
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr">
         <is>
-          <t>DayProfile (profile.py, 8); HourlyProfile (profile.py, 147); SUEWSConfig (core.py, 94); validate_hourly_profile_hours (core.py, 1802)</t>
+          <t>DayProfile (profile.py, 8); HourlyProfile (profile.py, 147); SUEWSConfig (core.py, 94); validate_hourly_profile_hours (core.py, 1838)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -3787,7 +3883,7 @@
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr">
         <is>
-          <t>DayProfile (profile.py, 8); HourlyProfile (profile.py, 147); SUEWSConfig (core.py, 94); validate_hourly_profile_hours (core.py, 1802)</t>
+          <t>DayProfile (profile.py, 8); HourlyProfile (profile.py, 147); SUEWSConfig (core.py, 94); validate_hourly_profile_hours (core.py, 1838)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -3811,7 +3907,7 @@
       <c r="B8" t="inlineStr"/>
       <c r="C8" t="inlineStr">
         <is>
-          <t>SUEWSConfig (core.py, 94); _check_co2_params (core.py, 672); CO2Params (human_activity.py, 339); YAMLAnnotator (yaml_annotator.py, 32); ValidationIssue (yaml_annotator_json.py, 16)</t>
+          <t>SUEWSConfig (core.py, 94); _check_co2_params (core.py, 694); CO2Params (human_activity.py, 339); YAMLAnnotator (yaml_annotator.py, 32); ValidationIssue (yaml_annotator_json.py, 16)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -3835,7 +3931,7 @@
       <c r="B9" t="inlineStr"/>
       <c r="C9" t="inlineStr">
         <is>
-          <t>SUEWSConfig (core.py, 94); _check_co2_params (core.py, 672); CO2Params (human_activity.py, 339); YAMLAnnotator (yaml_annotator.py, 32); ValidationIssue (yaml_annotator_json.py, 16)</t>
+          <t>SUEWSConfig (core.py, 94); _check_co2_params (core.py, 694); CO2Params (human_activity.py, 339); YAMLAnnotator (yaml_annotator.py, 32); ValidationIssue (yaml_annotator_json.py, 16)</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -5107,7 +5203,7 @@
       <c r="B62" t="inlineStr"/>
       <c r="C62" t="inlineStr">
         <is>
-          <t>DayProfile (profile.py, 8); HourlyProfile (profile.py, 147); SUEWSConfig (core.py, 94); validate_hourly_profile_hours (core.py, 1802)</t>
+          <t>DayProfile (profile.py, 8); HourlyProfile (profile.py, 147); SUEWSConfig (core.py, 94); validate_hourly_profile_hours (core.py, 1838)</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -5131,7 +5227,7 @@
       <c r="B63" t="inlineStr"/>
       <c r="C63" t="inlineStr">
         <is>
-          <t>DayProfile (profile.py, 8); HourlyProfile (profile.py, 147); SUEWSConfig (core.py, 94); validate_hourly_profile_hours (core.py, 1802)</t>
+          <t>DayProfile (profile.py, 8); HourlyProfile (profile.py, 147); SUEWSConfig (core.py, 94); validate_hourly_profile_hours (core.py, 1838)</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -6328,7 +6424,11 @@
           <t>anthropogenic_emissions.enddls</t>
         </is>
       </c>
-      <c r="B113" t="inlineStr"/>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
       <c r="C113" t="inlineStr">
         <is>
           <t>DLSCheck (precheck.py, 73); AnthropogenicEmissions (human_activity.py, 578)</t>
@@ -6355,7 +6455,7 @@
       <c r="B114" t="inlineStr"/>
       <c r="C114" t="inlineStr">
         <is>
-          <t>DayProfile (profile.py, 8); HourlyProfile (profile.py, 147); SUEWSConfig (core.py, 94); validate_hourly_profile_hours (core.py, 1802)</t>
+          <t>DayProfile (profile.py, 8); HourlyProfile (profile.py, 147); SUEWSConfig (core.py, 94); validate_hourly_profile_hours (core.py, 1838)</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
@@ -6379,7 +6479,7 @@
       <c r="B115" t="inlineStr"/>
       <c r="C115" t="inlineStr">
         <is>
-          <t>DayProfile (profile.py, 8); HourlyProfile (profile.py, 147); SUEWSConfig (core.py, 94); validate_hourly_profile_hours (core.py, 1802)</t>
+          <t>DayProfile (profile.py, 8); HourlyProfile (profile.py, 147); SUEWSConfig (core.py, 94); validate_hourly_profile_hours (core.py, 1838)</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
@@ -6403,7 +6503,7 @@
       <c r="B116" t="inlineStr"/>
       <c r="C116" t="inlineStr">
         <is>
-          <t>DayProfile (profile.py, 8); HourlyProfile (profile.py, 147); SUEWSConfig (core.py, 94); validate_hourly_profile_hours (core.py, 1802)</t>
+          <t>DayProfile (profile.py, 8); HourlyProfile (profile.py, 147); SUEWSConfig (core.py, 94); validate_hourly_profile_hours (core.py, 1838)</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
@@ -6427,7 +6527,7 @@
       <c r="B117" t="inlineStr"/>
       <c r="C117" t="inlineStr">
         <is>
-          <t>DayProfile (profile.py, 8); HourlyProfile (profile.py, 147); SUEWSConfig (core.py, 94); validate_hourly_profile_hours (core.py, 1802)</t>
+          <t>DayProfile (profile.py, 8); HourlyProfile (profile.py, 147); SUEWSConfig (core.py, 94); validate_hourly_profile_hours (core.py, 1838)</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
@@ -6451,7 +6551,7 @@
       <c r="B118" t="inlineStr"/>
       <c r="C118" t="inlineStr">
         <is>
-          <t>DayProfile (profile.py, 8); HourlyProfile (profile.py, 147); SUEWSConfig (core.py, 94); validate_hourly_profile_hours (core.py, 1802)</t>
+          <t>DayProfile (profile.py, 8); HourlyProfile (profile.py, 147); SUEWSConfig (core.py, 94); validate_hourly_profile_hours (core.py, 1838)</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
@@ -6475,7 +6575,7 @@
       <c r="B119" t="inlineStr"/>
       <c r="C119" t="inlineStr">
         <is>
-          <t>DayProfile (profile.py, 8); HourlyProfile (profile.py, 147); SUEWSConfig (core.py, 94); validate_hourly_profile_hours (core.py, 1802)</t>
+          <t>DayProfile (profile.py, 8); HourlyProfile (profile.py, 147); SUEWSConfig (core.py, 94); validate_hourly_profile_hours (core.py, 1838)</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
@@ -7651,7 +7751,7 @@
       <c r="B168" t="inlineStr"/>
       <c r="C168" t="inlineStr">
         <is>
-          <t>DayProfile (profile.py, 8); HourlyProfile (profile.py, 147); SUEWSConfig (core.py, 94); validate_hourly_profile_hours (core.py, 1802)</t>
+          <t>DayProfile (profile.py, 8); HourlyProfile (profile.py, 147); SUEWSConfig (core.py, 94); validate_hourly_profile_hours (core.py, 1838)</t>
         </is>
       </c>
       <c r="D168" t="inlineStr">
@@ -7675,7 +7775,7 @@
       <c r="B169" t="inlineStr"/>
       <c r="C169" t="inlineStr">
         <is>
-          <t>DayProfile (profile.py, 8); HourlyProfile (profile.py, 147); SUEWSConfig (core.py, 94); validate_hourly_profile_hours (core.py, 1802)</t>
+          <t>DayProfile (profile.py, 8); HourlyProfile (profile.py, 147); SUEWSConfig (core.py, 94); validate_hourly_profile_hours (core.py, 1838)</t>
         </is>
       </c>
       <c r="D169" t="inlineStr">
@@ -7699,7 +7799,7 @@
       <c r="B170" t="inlineStr"/>
       <c r="C170" t="inlineStr">
         <is>
-          <t>DayProfile (profile.py, 8); HourlyProfile (profile.py, 147); SUEWSConfig (core.py, 94); validate_hourly_profile_hours (core.py, 1802)</t>
+          <t>DayProfile (profile.py, 8); HourlyProfile (profile.py, 147); SUEWSConfig (core.py, 94); validate_hourly_profile_hours (core.py, 1838)</t>
         </is>
       </c>
       <c r="D170" t="inlineStr">
@@ -7723,7 +7823,7 @@
       <c r="B171" t="inlineStr"/>
       <c r="C171" t="inlineStr">
         <is>
-          <t>DayProfile (profile.py, 8); HourlyProfile (profile.py, 147); SUEWSConfig (core.py, 94); validate_hourly_profile_hours (core.py, 1802)</t>
+          <t>DayProfile (profile.py, 8); HourlyProfile (profile.py, 147); SUEWSConfig (core.py, 94); validate_hourly_profile_hours (core.py, 1838)</t>
         </is>
       </c>
       <c r="D171" t="inlineStr">
@@ -7747,7 +7847,7 @@
       <c r="B172" t="inlineStr"/>
       <c r="C172" t="inlineStr">
         <is>
-          <t>DayProfile (profile.py, 8); HourlyProfile (profile.py, 147); SUEWSConfig (core.py, 94); validate_hourly_profile_hours (core.py, 1802)</t>
+          <t>DayProfile (profile.py, 8); HourlyProfile (profile.py, 147); SUEWSConfig (core.py, 94); validate_hourly_profile_hours (core.py, 1838)</t>
         </is>
       </c>
       <c r="D172" t="inlineStr">
@@ -7771,7 +7871,7 @@
       <c r="B173" t="inlineStr"/>
       <c r="C173" t="inlineStr">
         <is>
-          <t>DayProfile (profile.py, 8); HourlyProfile (profile.py, 147); SUEWSConfig (core.py, 94); validate_hourly_profile_hours (core.py, 1802)</t>
+          <t>DayProfile (profile.py, 8); HourlyProfile (profile.py, 147); SUEWSConfig (core.py, 94); validate_hourly_profile_hours (core.py, 1838)</t>
         </is>
       </c>
       <c r="D173" t="inlineStr">
@@ -8971,7 +9071,7 @@
       <c r="B223" t="inlineStr"/>
       <c r="C223" t="inlineStr">
         <is>
-          <t>DayProfile (profile.py, 8); HourlyProfile (profile.py, 147); SUEWSConfig (core.py, 94); validate_hourly_profile_hours (core.py, 1802)</t>
+          <t>DayProfile (profile.py, 8); HourlyProfile (profile.py, 147); SUEWSConfig (core.py, 94); validate_hourly_profile_hours (core.py, 1838)</t>
         </is>
       </c>
       <c r="D223" t="inlineStr">
@@ -8995,7 +9095,7 @@
       <c r="B224" t="inlineStr"/>
       <c r="C224" t="inlineStr">
         <is>
-          <t>DayProfile (profile.py, 8); HourlyProfile (profile.py, 147); SUEWSConfig (core.py, 94); validate_hourly_profile_hours (core.py, 1802)</t>
+          <t>DayProfile (profile.py, 8); HourlyProfile (profile.py, 147); SUEWSConfig (core.py, 94); validate_hourly_profile_hours (core.py, 1838)</t>
         </is>
       </c>
       <c r="D224" t="inlineStr">
@@ -9019,7 +9119,7 @@
       <c r="B225" t="inlineStr"/>
       <c r="C225" t="inlineStr">
         <is>
-          <t>DayProfile (profile.py, 8); HourlyProfile (profile.py, 147); SUEWSConfig (core.py, 94); validate_hourly_profile_hours (core.py, 1802)</t>
+          <t>DayProfile (profile.py, 8); HourlyProfile (profile.py, 147); SUEWSConfig (core.py, 94); validate_hourly_profile_hours (core.py, 1838)</t>
         </is>
       </c>
       <c r="D225" t="inlineStr">
@@ -9043,7 +9143,7 @@
       <c r="B226" t="inlineStr"/>
       <c r="C226" t="inlineStr">
         <is>
-          <t>DayProfile (profile.py, 8); HourlyProfile (profile.py, 147); SUEWSConfig (core.py, 94); validate_hourly_profile_hours (core.py, 1802)</t>
+          <t>DayProfile (profile.py, 8); HourlyProfile (profile.py, 147); SUEWSConfig (core.py, 94); validate_hourly_profile_hours (core.py, 1838)</t>
         </is>
       </c>
       <c r="D226" t="inlineStr">
@@ -9067,7 +9167,7 @@
       <c r="B227" t="inlineStr"/>
       <c r="C227" t="inlineStr">
         <is>
-          <t>DayProfile (profile.py, 8); HourlyProfile (profile.py, 147); SUEWSConfig (core.py, 94); validate_hourly_profile_hours (core.py, 1802)</t>
+          <t>DayProfile (profile.py, 8); HourlyProfile (profile.py, 147); SUEWSConfig (core.py, 94); validate_hourly_profile_hours (core.py, 1838)</t>
         </is>
       </c>
       <c r="D227" t="inlineStr">
@@ -9091,7 +9191,7 @@
       <c r="B228" t="inlineStr"/>
       <c r="C228" t="inlineStr">
         <is>
-          <t>DayProfile (profile.py, 8); HourlyProfile (profile.py, 147); SUEWSConfig (core.py, 94); validate_hourly_profile_hours (core.py, 1802)</t>
+          <t>DayProfile (profile.py, 8); HourlyProfile (profile.py, 147); SUEWSConfig (core.py, 94); validate_hourly_profile_hours (core.py, 1838)</t>
         </is>
       </c>
       <c r="D228" t="inlineStr">
@@ -9115,7 +9215,7 @@
       <c r="B229" t="inlineStr"/>
       <c r="C229" t="inlineStr">
         <is>
-          <t>DayProfile (profile.py, 8); HourlyProfile (profile.py, 147); SUEWSConfig (core.py, 94); validate_hourly_profile_hours (core.py, 1802)</t>
+          <t>DayProfile (profile.py, 8); HourlyProfile (profile.py, 147); SUEWSConfig (core.py, 94); validate_hourly_profile_hours (core.py, 1838)</t>
         </is>
       </c>
       <c r="D229" t="inlineStr">
@@ -9139,7 +9239,7 @@
       <c r="B230" t="inlineStr"/>
       <c r="C230" t="inlineStr">
         <is>
-          <t>DayProfile (profile.py, 8); HourlyProfile (profile.py, 147); SUEWSConfig (core.py, 94); validate_hourly_profile_hours (core.py, 1802)</t>
+          <t>DayProfile (profile.py, 8); HourlyProfile (profile.py, 147); SUEWSConfig (core.py, 94); validate_hourly_profile_hours (core.py, 1838)</t>
         </is>
       </c>
       <c r="D230" t="inlineStr">
@@ -10147,7 +10247,7 @@
       <c r="B272" t="inlineStr"/>
       <c r="C272" t="inlineStr">
         <is>
-          <t>SUEWSConfig (core.py, 94); _check_conductance (core.py, 645); Conductance (site.py, 68); YAMLAnnotator (yaml_annotator.py, 32); ValidationIssue (yaml_annotator_json.py, 16)</t>
+          <t>SUEWSConfig (core.py, 94); _check_conductance (core.py, 667); Conductance (site.py, 68); YAMLAnnotator (yaml_annotator.py, 32); ValidationIssue (yaml_annotator_json.py, 16)</t>
         </is>
       </c>
       <c r="D272" t="inlineStr">
@@ -10171,7 +10271,7 @@
       <c r="B273" t="inlineStr"/>
       <c r="C273" t="inlineStr">
         <is>
-          <t>SUEWSConfig (core.py, 94); _check_conductance (core.py, 645); Conductance (site.py, 68); YAMLAnnotator (yaml_annotator.py, 32); ValidationIssue (yaml_annotator_json.py, 16)</t>
+          <t>SUEWSConfig (core.py, 94); _check_conductance (core.py, 667); Conductance (site.py, 68); YAMLAnnotator (yaml_annotator.py, 32); ValidationIssue (yaml_annotator_json.py, 16)</t>
         </is>
       </c>
       <c r="D273" t="inlineStr">
@@ -10243,7 +10343,7 @@
       <c r="B276" t="inlineStr"/>
       <c r="C276" t="inlineStr">
         <is>
-          <t>SUEWSConfig (core.py, 94); _check_conductance (core.py, 645); Conductance (site.py, 68); YAMLAnnotator (yaml_annotator.py, 32); ValidationIssue (yaml_annotator_json.py, 16)</t>
+          <t>SUEWSConfig (core.py, 94); _check_conductance (core.py, 667); Conductance (site.py, 68); YAMLAnnotator (yaml_annotator.py, 32); ValidationIssue (yaml_annotator_json.py, 16)</t>
         </is>
       </c>
       <c r="D276" t="inlineStr">
@@ -13267,7 +13367,7 @@
       <c r="B402" t="inlineStr"/>
       <c r="C402" t="inlineStr">
         <is>
-          <t>SUEWSConfig (core.py, 94); _check_surface_parameters (core.py, 710); validate_only_when_complete (validation_utils.py, 122); YAMLAnnotator (yaml_annotator.py, 32); ValidationIssue (yaml_annotator_json.py, 16); BldgsProperties (surface.py, 818)</t>
+          <t>SUEWSConfig (core.py, 94); _check_surface_parameters (core.py, 732); validate_only_when_complete (validation_utils.py, 122); YAMLAnnotator (yaml_annotator.py, 32); ValidationIssue (yaml_annotator_json.py, 16); BldgsProperties (surface.py, 818)</t>
         </is>
       </c>
       <c r="D402" t="inlineStr">
@@ -13363,7 +13463,7 @@
       <c r="B406" t="inlineStr"/>
       <c r="C406" t="inlineStr">
         <is>
-          <t>SUEWSConfig (core.py, 94); _check_surface_parameters (core.py, 710); _validate_rsl (core.py, 1101); validate_only_when_complete (validation_utils.py, 122); YAMLAnnotator (yaml_annotator.py, 32); ValidationIssue (yaml_annotator_json.py, 16); BldgsProperties (surface.py, 818); validate_rsl_zd_range (surface.py, 844)</t>
+          <t>SUEWSConfig (core.py, 94); _check_surface_parameters (core.py, 732); _validate_rsl (core.py, 1123); validate_only_when_complete (validation_utils.py, 122); YAMLAnnotator (yaml_annotator.py, 32); ValidationIssue (yaml_annotator_json.py, 16); BldgsProperties (surface.py, 818); validate_rsl_zd_range (surface.py, 844)</t>
         </is>
       </c>
       <c r="D406" t="inlineStr">
@@ -13795,7 +13895,7 @@
       <c r="B424" t="inlineStr"/>
       <c r="C424" t="inlineStr">
         <is>
-          <t>SUEWSConfig (core.py, 94); _check_surface_parameters (core.py, 710); _check_land_cover_fractions (core.py, 889); _validate_rsl (core.py, 1101); validate_only_when_complete (validation_utils.py, 122); check_recursively (precheck.py, 949); SurfaceProperties (surface.py, 159); validate_rsl_zd_range (surface.py, 844)</t>
+          <t>SUEWSConfig (core.py, 94); _check_surface_parameters (core.py, 732); _check_land_cover_fractions (core.py, 911); _validate_rsl (core.py, 1123); validate_only_when_complete (validation_utils.py, 122); check_recursively (precheck.py, 949); SurfaceProperties (surface.py, 159); validate_rsl_zd_range (surface.py, 844)</t>
         </is>
       </c>
       <c r="D424" t="inlineStr">
@@ -13868,7 +13968,11 @@
           <t>land_cover.bldgs.soilstorecap</t>
         </is>
       </c>
-      <c r="B427" t="inlineStr"/>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
       <c r="C427" t="inlineStr">
         <is>
           <t>SurfaceProperties (surface.py, 159); BuildingLayer (surface.py, 637)</t>
@@ -13892,7 +13996,11 @@
           <t>land_cover.bldgs.statelimit</t>
         </is>
       </c>
-      <c r="B428" t="inlineStr"/>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
       <c r="C428" t="inlineStr">
         <is>
           <t>SurfaceProperties (surface.py, 159); BuildingLayer (surface.py, 637)</t>
@@ -14111,7 +14219,7 @@
       <c r="B437" t="inlineStr"/>
       <c r="C437" t="inlineStr">
         <is>
-          <t>SUEWSConfig (core.py, 94); _check_thermal_layers (core.py, 770); _validate_storage (core.py, 1144); YAMLAnnotator (yaml_annotator.py, 32); ValidationIssue (yaml_annotator_json.py, 16); ThermalLayers (surface.py, 25)</t>
+          <t>SUEWSConfig (core.py, 94); _check_thermal_layers (core.py, 792); _validate_storage (core.py, 1166); YAMLAnnotator (yaml_annotator.py, 32); ValidationIssue (yaml_annotator_json.py, 16); ThermalLayers (surface.py, 25)</t>
         </is>
       </c>
       <c r="D437" t="inlineStr">
@@ -14831,7 +14939,7 @@
       <c r="B467" t="inlineStr"/>
       <c r="C467" t="inlineStr">
         <is>
-          <t>SUEWSConfig (core.py, 94); _check_surface_parameters (core.py, 710); _check_land_cover_fractions (core.py, 889); _validate_rsl (core.py, 1101); validate_only_when_complete (validation_utils.py, 122); check_recursively (precheck.py, 949); SurfaceProperties (surface.py, 159); validate_rsl_zd_range (surface.py, 844)</t>
+          <t>SUEWSConfig (core.py, 94); _check_surface_parameters (core.py, 732); _check_land_cover_fractions (core.py, 911); _validate_rsl (core.py, 1123); validate_only_when_complete (validation_utils.py, 122); check_recursively (precheck.py, 949); SurfaceProperties (surface.py, 159); validate_rsl_zd_range (surface.py, 844)</t>
         </is>
       </c>
       <c r="D467" t="inlineStr">
@@ -14904,7 +15012,11 @@
           <t>land_cover.bsoil.soilstorecap</t>
         </is>
       </c>
-      <c r="B470" t="inlineStr"/>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
       <c r="C470" t="inlineStr">
         <is>
           <t>SurfaceProperties (surface.py, 159); BuildingLayer (surface.py, 637)</t>
@@ -14928,7 +15040,11 @@
           <t>land_cover.bsoil.statelimit</t>
         </is>
       </c>
-      <c r="B471" t="inlineStr"/>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
       <c r="C471" t="inlineStr">
         <is>
           <t>SurfaceProperties (surface.py, 159); BuildingLayer (surface.py, 637)</t>
@@ -15147,7 +15263,7 @@
       <c r="B480" t="inlineStr"/>
       <c r="C480" t="inlineStr">
         <is>
-          <t>SUEWSConfig (core.py, 94); _check_thermal_layers (core.py, 770); _validate_storage (core.py, 1144); YAMLAnnotator (yaml_annotator.py, 32); ValidationIssue (yaml_annotator_json.py, 16); ThermalLayers (surface.py, 25)</t>
+          <t>SUEWSConfig (core.py, 94); _check_thermal_layers (core.py, 792); _validate_storage (core.py, 1166); YAMLAnnotator (yaml_annotator.py, 32); ValidationIssue (yaml_annotator_json.py, 16); ThermalLayers (surface.py, 25)</t>
         </is>
       </c>
       <c r="D480" t="inlineStr">
@@ -15435,7 +15551,7 @@
       <c r="B492" t="inlineStr"/>
       <c r="C492" t="inlineStr">
         <is>
-          <t>SUEWSConfig (core.py, 94); _check_surface_parameters (core.py, 710); VegetatedSurfaceProperties (site.py, 433)</t>
+          <t>SUEWSConfig (core.py, 94); _check_surface_parameters (core.py, 732); VegetatedSurfaceProperties (site.py, 433)</t>
         </is>
       </c>
       <c r="D492" t="inlineStr">
@@ -15483,7 +15599,7 @@
       <c r="B494" t="inlineStr"/>
       <c r="C494" t="inlineStr">
         <is>
-          <t>SUEWSConfig (core.py, 94); _check_surface_parameters (core.py, 710); VegetatedSurfaceProperties (site.py, 433)</t>
+          <t>SUEWSConfig (core.py, 94); _check_surface_parameters (core.py, 732); VegetatedSurfaceProperties (site.py, 433)</t>
         </is>
       </c>
       <c r="D494" t="inlineStr">
@@ -15795,7 +15911,7 @@
       <c r="B507" t="inlineStr"/>
       <c r="C507" t="inlineStr">
         <is>
-          <t>_check_lai_ranges (core.py, 804); LAIParams (site.py, 287)</t>
+          <t>_check_lai_ranges (core.py, 826); LAIParams (site.py, 287)</t>
         </is>
       </c>
       <c r="D507" t="inlineStr">
@@ -15840,10 +15956,14 @@
           <t>land_cover.dectr.lai.gddfull</t>
         </is>
       </c>
-      <c r="B509" t="inlineStr"/>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
       <c r="C509" t="inlineStr">
         <is>
-          <t>_check_lai_ranges (core.py, 804); LAIParams (site.py, 287)</t>
+          <t>_check_lai_ranges (core.py, 826); LAIParams (site.py, 287)</t>
         </is>
       </c>
       <c r="D509" t="inlineStr">
@@ -15867,7 +15987,7 @@
       <c r="B510" t="inlineStr"/>
       <c r="C510" t="inlineStr">
         <is>
-          <t>_check_lai_ranges (core.py, 804); LAIParams (site.py, 287)</t>
+          <t>_check_lai_ranges (core.py, 826); LAIParams (site.py, 287)</t>
         </is>
       </c>
       <c r="D510" t="inlineStr">
@@ -15891,7 +16011,7 @@
       <c r="B511" t="inlineStr"/>
       <c r="C511" t="inlineStr">
         <is>
-          <t>_check_lai_ranges (core.py, 804); LAIParams (site.py, 287)</t>
+          <t>_check_lai_ranges (core.py, 826); LAIParams (site.py, 287)</t>
         </is>
       </c>
       <c r="D511" t="inlineStr">
@@ -15912,7 +16032,11 @@
           <t>land_cover.dectr.lai.laipower.growth_gdd</t>
         </is>
       </c>
-      <c r="B512" t="inlineStr"/>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
       <c r="C512" t="inlineStr">
         <is>
           <t>LAIPowerCoefficients (site.py, 195)</t>
@@ -15984,7 +16108,11 @@
           <t>land_cover.dectr.lai.laipower.senescence_sdd</t>
         </is>
       </c>
-      <c r="B515" t="inlineStr"/>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
       <c r="C515" t="inlineStr">
         <is>
           <t>LAIPowerCoefficients (site.py, 195)</t>
@@ -16032,7 +16160,11 @@
           <t>land_cover.dectr.lai.sddfull</t>
         </is>
       </c>
-      <c r="B517" t="inlineStr"/>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
       <c r="C517" t="inlineStr">
         <is>
           <t>LAIParams (site.py, 287)</t>
@@ -16491,7 +16623,7 @@
       <c r="B536" t="inlineStr"/>
       <c r="C536" t="inlineStr">
         <is>
-          <t>SUEWSConfig (core.py, 94); _check_surface_parameters (core.py, 710); VegetatedSurfaceProperties (site.py, 433)</t>
+          <t>SUEWSConfig (core.py, 94); _check_surface_parameters (core.py, 732); VegetatedSurfaceProperties (site.py, 433)</t>
         </is>
       </c>
       <c r="D536" t="inlineStr">
@@ -16515,7 +16647,7 @@
       <c r="B537" t="inlineStr"/>
       <c r="C537" t="inlineStr">
         <is>
-          <t>SUEWSConfig (core.py, 94); _check_surface_parameters (core.py, 710); VegetatedSurfaceProperties (site.py, 433)</t>
+          <t>SUEWSConfig (core.py, 94); _check_surface_parameters (core.py, 732); VegetatedSurfaceProperties (site.py, 433)</t>
         </is>
       </c>
       <c r="D537" t="inlineStr">
@@ -16563,7 +16695,7 @@
       <c r="B539" t="inlineStr"/>
       <c r="C539" t="inlineStr">
         <is>
-          <t>SUEWSConfig (core.py, 94); _check_surface_parameters (core.py, 710); _check_land_cover_fractions (core.py, 889); _validate_rsl (core.py, 1101); validate_only_when_complete (validation_utils.py, 122); check_recursively (precheck.py, 949); SurfaceProperties (surface.py, 159); validate_rsl_zd_range (surface.py, 844)</t>
+          <t>SUEWSConfig (core.py, 94); _check_surface_parameters (core.py, 732); _check_land_cover_fractions (core.py, 911); _validate_rsl (core.py, 1123); validate_only_when_complete (validation_utils.py, 122); check_recursively (precheck.py, 949); SurfaceProperties (surface.py, 159); validate_rsl_zd_range (surface.py, 844)</t>
         </is>
       </c>
       <c r="D539" t="inlineStr">
@@ -16636,7 +16768,11 @@
           <t>land_cover.dectr.soilstorecap</t>
         </is>
       </c>
-      <c r="B542" t="inlineStr"/>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
       <c r="C542" t="inlineStr">
         <is>
           <t>SurfaceProperties (surface.py, 159); BuildingLayer (surface.py, 637)</t>
@@ -16660,7 +16796,11 @@
           <t>land_cover.dectr.statelimit</t>
         </is>
       </c>
-      <c r="B543" t="inlineStr"/>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
       <c r="C543" t="inlineStr">
         <is>
           <t>SurfaceProperties (surface.py, 159); BuildingLayer (surface.py, 637)</t>
@@ -16879,7 +17019,7 @@
       <c r="B552" t="inlineStr"/>
       <c r="C552" t="inlineStr">
         <is>
-          <t>SUEWSConfig (core.py, 94); _check_thermal_layers (core.py, 770); _validate_storage (core.py, 1144); YAMLAnnotator (yaml_annotator.py, 32); ValidationIssue (yaml_annotator_json.py, 16); ThermalLayers (surface.py, 25)</t>
+          <t>SUEWSConfig (core.py, 94); _check_thermal_layers (core.py, 792); _validate_storage (core.py, 1166); YAMLAnnotator (yaml_annotator.py, 32); ValidationIssue (yaml_annotator_json.py, 16); ThermalLayers (surface.py, 25)</t>
         </is>
       </c>
       <c r="D552" t="inlineStr">
@@ -17191,7 +17331,7 @@
       <c r="B565" t="inlineStr"/>
       <c r="C565" t="inlineStr">
         <is>
-          <t>SUEWSConfig (core.py, 94); _check_surface_parameters (core.py, 710); VegetatedSurfaceProperties (site.py, 433)</t>
+          <t>SUEWSConfig (core.py, 94); _check_surface_parameters (core.py, 732); VegetatedSurfaceProperties (site.py, 433)</t>
         </is>
       </c>
       <c r="D565" t="inlineStr">
@@ -17239,7 +17379,7 @@
       <c r="B567" t="inlineStr"/>
       <c r="C567" t="inlineStr">
         <is>
-          <t>SUEWSConfig (core.py, 94); _check_surface_parameters (core.py, 710); VegetatedSurfaceProperties (site.py, 433)</t>
+          <t>SUEWSConfig (core.py, 94); _check_surface_parameters (core.py, 732); VegetatedSurfaceProperties (site.py, 433)</t>
         </is>
       </c>
       <c r="D567" t="inlineStr">
@@ -17503,7 +17643,7 @@
       <c r="B578" t="inlineStr"/>
       <c r="C578" t="inlineStr">
         <is>
-          <t>_check_lai_ranges (core.py, 804); LAIParams (site.py, 287)</t>
+          <t>_check_lai_ranges (core.py, 826); LAIParams (site.py, 287)</t>
         </is>
       </c>
       <c r="D578" t="inlineStr">
@@ -17548,10 +17688,14 @@
           <t>land_cover.evetr.lai.gddfull</t>
         </is>
       </c>
-      <c r="B580" t="inlineStr"/>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
       <c r="C580" t="inlineStr">
         <is>
-          <t>_check_lai_ranges (core.py, 804); LAIParams (site.py, 287)</t>
+          <t>_check_lai_ranges (core.py, 826); LAIParams (site.py, 287)</t>
         </is>
       </c>
       <c r="D580" t="inlineStr">
@@ -17575,7 +17719,7 @@
       <c r="B581" t="inlineStr"/>
       <c r="C581" t="inlineStr">
         <is>
-          <t>_check_lai_ranges (core.py, 804); LAIParams (site.py, 287)</t>
+          <t>_check_lai_ranges (core.py, 826); LAIParams (site.py, 287)</t>
         </is>
       </c>
       <c r="D581" t="inlineStr">
@@ -17599,7 +17743,7 @@
       <c r="B582" t="inlineStr"/>
       <c r="C582" t="inlineStr">
         <is>
-          <t>_check_lai_ranges (core.py, 804); LAIParams (site.py, 287)</t>
+          <t>_check_lai_ranges (core.py, 826); LAIParams (site.py, 287)</t>
         </is>
       </c>
       <c r="D582" t="inlineStr">
@@ -17620,7 +17764,11 @@
           <t>land_cover.evetr.lai.laipower.growth_gdd</t>
         </is>
       </c>
-      <c r="B583" t="inlineStr"/>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
       <c r="C583" t="inlineStr">
         <is>
           <t>LAIPowerCoefficients (site.py, 195)</t>
@@ -17692,7 +17840,11 @@
           <t>land_cover.evetr.lai.laipower.senescence_sdd</t>
         </is>
       </c>
-      <c r="B586" t="inlineStr"/>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
       <c r="C586" t="inlineStr">
         <is>
           <t>LAIPowerCoefficients (site.py, 195)</t>
@@ -17740,7 +17892,11 @@
           <t>land_cover.evetr.lai.sddfull</t>
         </is>
       </c>
-      <c r="B588" t="inlineStr"/>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
       <c r="C588" t="inlineStr">
         <is>
           <t>LAIParams (site.py, 287)</t>
@@ -18151,7 +18307,7 @@
       <c r="B605" t="inlineStr"/>
       <c r="C605" t="inlineStr">
         <is>
-          <t>SUEWSConfig (core.py, 94); _check_surface_parameters (core.py, 710); VegetatedSurfaceProperties (site.py, 433)</t>
+          <t>SUEWSConfig (core.py, 94); _check_surface_parameters (core.py, 732); VegetatedSurfaceProperties (site.py, 433)</t>
         </is>
       </c>
       <c r="D605" t="inlineStr">
@@ -18175,7 +18331,7 @@
       <c r="B606" t="inlineStr"/>
       <c r="C606" t="inlineStr">
         <is>
-          <t>SUEWSConfig (core.py, 94); _check_surface_parameters (core.py, 710); VegetatedSurfaceProperties (site.py, 433)</t>
+          <t>SUEWSConfig (core.py, 94); _check_surface_parameters (core.py, 732); VegetatedSurfaceProperties (site.py, 433)</t>
         </is>
       </c>
       <c r="D606" t="inlineStr">
@@ -18223,7 +18379,7 @@
       <c r="B608" t="inlineStr"/>
       <c r="C608" t="inlineStr">
         <is>
-          <t>SUEWSConfig (core.py, 94); _check_surface_parameters (core.py, 710); _check_land_cover_fractions (core.py, 889); _validate_rsl (core.py, 1101); validate_only_when_complete (validation_utils.py, 122); check_recursively (precheck.py, 949); SurfaceProperties (surface.py, 159); validate_rsl_zd_range (surface.py, 844)</t>
+          <t>SUEWSConfig (core.py, 94); _check_surface_parameters (core.py, 732); _check_land_cover_fractions (core.py, 911); _validate_rsl (core.py, 1123); validate_only_when_complete (validation_utils.py, 122); check_recursively (precheck.py, 949); SurfaceProperties (surface.py, 159); validate_rsl_zd_range (surface.py, 844)</t>
         </is>
       </c>
       <c r="D608" t="inlineStr">
@@ -18296,7 +18452,11 @@
           <t>land_cover.evetr.soilstorecap</t>
         </is>
       </c>
-      <c r="B611" t="inlineStr"/>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
       <c r="C611" t="inlineStr">
         <is>
           <t>SurfaceProperties (surface.py, 159); BuildingLayer (surface.py, 637)</t>
@@ -18320,7 +18480,11 @@
           <t>land_cover.evetr.statelimit</t>
         </is>
       </c>
-      <c r="B612" t="inlineStr"/>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
       <c r="C612" t="inlineStr">
         <is>
           <t>SurfaceProperties (surface.py, 159); BuildingLayer (surface.py, 637)</t>
@@ -18539,7 +18703,7 @@
       <c r="B621" t="inlineStr"/>
       <c r="C621" t="inlineStr">
         <is>
-          <t>SUEWSConfig (core.py, 94); _check_thermal_layers (core.py, 770); _validate_storage (core.py, 1144); YAMLAnnotator (yaml_annotator.py, 32); ValidationIssue (yaml_annotator_json.py, 16); ThermalLayers (surface.py, 25)</t>
+          <t>SUEWSConfig (core.py, 94); _check_thermal_layers (core.py, 792); _validate_storage (core.py, 1166); YAMLAnnotator (yaml_annotator.py, 32); ValidationIssue (yaml_annotator_json.py, 16); ThermalLayers (surface.py, 25)</t>
         </is>
       </c>
       <c r="D621" t="inlineStr">
@@ -18851,7 +19015,7 @@
       <c r="B634" t="inlineStr"/>
       <c r="C634" t="inlineStr">
         <is>
-          <t>SUEWSConfig (core.py, 94); _check_surface_parameters (core.py, 710); VegetatedSurfaceProperties (site.py, 433)</t>
+          <t>SUEWSConfig (core.py, 94); _check_surface_parameters (core.py, 732); VegetatedSurfaceProperties (site.py, 433)</t>
         </is>
       </c>
       <c r="D634" t="inlineStr">
@@ -18899,7 +19063,7 @@
       <c r="B636" t="inlineStr"/>
       <c r="C636" t="inlineStr">
         <is>
-          <t>SUEWSConfig (core.py, 94); _check_surface_parameters (core.py, 710); VegetatedSurfaceProperties (site.py, 433)</t>
+          <t>SUEWSConfig (core.py, 94); _check_surface_parameters (core.py, 732); VegetatedSurfaceProperties (site.py, 433)</t>
         </is>
       </c>
       <c r="D636" t="inlineStr">
@@ -19115,7 +19279,7 @@
       <c r="B645" t="inlineStr"/>
       <c r="C645" t="inlineStr">
         <is>
-          <t>_check_lai_ranges (core.py, 804); LAIParams (site.py, 287)</t>
+          <t>_check_lai_ranges (core.py, 826); LAIParams (site.py, 287)</t>
         </is>
       </c>
       <c r="D645" t="inlineStr">
@@ -19160,10 +19324,14 @@
           <t>land_cover.grass.lai.gddfull</t>
         </is>
       </c>
-      <c r="B647" t="inlineStr"/>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
       <c r="C647" t="inlineStr">
         <is>
-          <t>_check_lai_ranges (core.py, 804); LAIParams (site.py, 287)</t>
+          <t>_check_lai_ranges (core.py, 826); LAIParams (site.py, 287)</t>
         </is>
       </c>
       <c r="D647" t="inlineStr">
@@ -19187,7 +19355,7 @@
       <c r="B648" t="inlineStr"/>
       <c r="C648" t="inlineStr">
         <is>
-          <t>_check_lai_ranges (core.py, 804); LAIParams (site.py, 287)</t>
+          <t>_check_lai_ranges (core.py, 826); LAIParams (site.py, 287)</t>
         </is>
       </c>
       <c r="D648" t="inlineStr">
@@ -19211,7 +19379,7 @@
       <c r="B649" t="inlineStr"/>
       <c r="C649" t="inlineStr">
         <is>
-          <t>_check_lai_ranges (core.py, 804); LAIParams (site.py, 287)</t>
+          <t>_check_lai_ranges (core.py, 826); LAIParams (site.py, 287)</t>
         </is>
       </c>
       <c r="D649" t="inlineStr">
@@ -19232,7 +19400,11 @@
           <t>land_cover.grass.lai.laipower.growth_gdd</t>
         </is>
       </c>
-      <c r="B650" t="inlineStr"/>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
       <c r="C650" t="inlineStr">
         <is>
           <t>LAIPowerCoefficients (site.py, 195)</t>
@@ -19304,7 +19476,11 @@
           <t>land_cover.grass.lai.laipower.senescence_sdd</t>
         </is>
       </c>
-      <c r="B653" t="inlineStr"/>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
       <c r="C653" t="inlineStr">
         <is>
           <t>LAIPowerCoefficients (site.py, 195)</t>
@@ -19352,7 +19528,11 @@
           <t>land_cover.grass.lai.sddfull</t>
         </is>
       </c>
-      <c r="B655" t="inlineStr"/>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
       <c r="C655" t="inlineStr">
         <is>
           <t>LAIParams (site.py, 287)</t>
@@ -19763,7 +19943,7 @@
       <c r="B672" t="inlineStr"/>
       <c r="C672" t="inlineStr">
         <is>
-          <t>SUEWSConfig (core.py, 94); _check_surface_parameters (core.py, 710); VegetatedSurfaceProperties (site.py, 433)</t>
+          <t>SUEWSConfig (core.py, 94); _check_surface_parameters (core.py, 732); VegetatedSurfaceProperties (site.py, 433)</t>
         </is>
       </c>
       <c r="D672" t="inlineStr">
@@ -19787,7 +19967,7 @@
       <c r="B673" t="inlineStr"/>
       <c r="C673" t="inlineStr">
         <is>
-          <t>SUEWSConfig (core.py, 94); _check_surface_parameters (core.py, 710); VegetatedSurfaceProperties (site.py, 433)</t>
+          <t>SUEWSConfig (core.py, 94); _check_surface_parameters (core.py, 732); VegetatedSurfaceProperties (site.py, 433)</t>
         </is>
       </c>
       <c r="D673" t="inlineStr">
@@ -19835,7 +20015,7 @@
       <c r="B675" t="inlineStr"/>
       <c r="C675" t="inlineStr">
         <is>
-          <t>SUEWSConfig (core.py, 94); _check_surface_parameters (core.py, 710); _check_land_cover_fractions (core.py, 889); _validate_rsl (core.py, 1101); validate_only_when_complete (validation_utils.py, 122); check_recursively (precheck.py, 949); SurfaceProperties (surface.py, 159); validate_rsl_zd_range (surface.py, 844)</t>
+          <t>SUEWSConfig (core.py, 94); _check_surface_parameters (core.py, 732); _check_land_cover_fractions (core.py, 911); _validate_rsl (core.py, 1123); validate_only_when_complete (validation_utils.py, 122); check_recursively (precheck.py, 949); SurfaceProperties (surface.py, 159); validate_rsl_zd_range (surface.py, 844)</t>
         </is>
       </c>
       <c r="D675" t="inlineStr">
@@ -19908,7 +20088,11 @@
           <t>land_cover.grass.soilstorecap</t>
         </is>
       </c>
-      <c r="B678" t="inlineStr"/>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
       <c r="C678" t="inlineStr">
         <is>
           <t>SurfaceProperties (surface.py, 159); BuildingLayer (surface.py, 637)</t>
@@ -19932,7 +20116,11 @@
           <t>land_cover.grass.statelimit</t>
         </is>
       </c>
-      <c r="B679" t="inlineStr"/>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
       <c r="C679" t="inlineStr">
         <is>
           <t>SurfaceProperties (surface.py, 159); BuildingLayer (surface.py, 637)</t>
@@ -20151,7 +20339,7 @@
       <c r="B688" t="inlineStr"/>
       <c r="C688" t="inlineStr">
         <is>
-          <t>SUEWSConfig (core.py, 94); _check_thermal_layers (core.py, 770); _validate_storage (core.py, 1144); YAMLAnnotator (yaml_annotator.py, 32); ValidationIssue (yaml_annotator_json.py, 16); ThermalLayers (surface.py, 25)</t>
+          <t>SUEWSConfig (core.py, 94); _check_thermal_layers (core.py, 792); _validate_storage (core.py, 1166); YAMLAnnotator (yaml_annotator.py, 32); ValidationIssue (yaml_annotator_json.py, 16); ThermalLayers (surface.py, 25)</t>
         </is>
       </c>
       <c r="D688" t="inlineStr">
@@ -20895,7 +21083,7 @@
       <c r="B719" t="inlineStr"/>
       <c r="C719" t="inlineStr">
         <is>
-          <t>SUEWSConfig (core.py, 94); _check_surface_parameters (core.py, 710); _check_land_cover_fractions (core.py, 889); _validate_rsl (core.py, 1101); validate_only_when_complete (validation_utils.py, 122); check_recursively (precheck.py, 949); SurfaceProperties (surface.py, 159); validate_rsl_zd_range (surface.py, 844)</t>
+          <t>SUEWSConfig (core.py, 94); _check_surface_parameters (core.py, 732); _check_land_cover_fractions (core.py, 911); _validate_rsl (core.py, 1123); validate_only_when_complete (validation_utils.py, 122); check_recursively (precheck.py, 949); SurfaceProperties (surface.py, 159); validate_rsl_zd_range (surface.py, 844)</t>
         </is>
       </c>
       <c r="D719" t="inlineStr">
@@ -20968,7 +21156,11 @@
           <t>land_cover.paved.soilstorecap</t>
         </is>
       </c>
-      <c r="B722" t="inlineStr"/>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
       <c r="C722" t="inlineStr">
         <is>
           <t>SurfaceProperties (surface.py, 159); BuildingLayer (surface.py, 637)</t>
@@ -20992,7 +21184,11 @@
           <t>land_cover.paved.statelimit</t>
         </is>
       </c>
-      <c r="B723" t="inlineStr"/>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
       <c r="C723" t="inlineStr">
         <is>
           <t>SurfaceProperties (surface.py, 159); BuildingLayer (surface.py, 637)</t>
@@ -21211,7 +21407,7 @@
       <c r="B732" t="inlineStr"/>
       <c r="C732" t="inlineStr">
         <is>
-          <t>SUEWSConfig (core.py, 94); _check_thermal_layers (core.py, 770); _validate_storage (core.py, 1144); YAMLAnnotator (yaml_annotator.py, 32); ValidationIssue (yaml_annotator_json.py, 16); ThermalLayers (surface.py, 25)</t>
+          <t>SUEWSConfig (core.py, 94); _check_thermal_layers (core.py, 792); _validate_storage (core.py, 1166); YAMLAnnotator (yaml_annotator.py, 32); ValidationIssue (yaml_annotator_json.py, 16); ThermalLayers (surface.py, 25)</t>
         </is>
       </c>
       <c r="D732" t="inlineStr">
@@ -21955,7 +22151,7 @@
       <c r="B763" t="inlineStr"/>
       <c r="C763" t="inlineStr">
         <is>
-          <t>SUEWSConfig (core.py, 94); _check_surface_parameters (core.py, 710); _check_land_cover_fractions (core.py, 889); _validate_rsl (core.py, 1101); validate_only_when_complete (validation_utils.py, 122); check_recursively (precheck.py, 949); SurfaceProperties (surface.py, 159); validate_rsl_zd_range (surface.py, 844)</t>
+          <t>SUEWSConfig (core.py, 94); _check_surface_parameters (core.py, 732); _check_land_cover_fractions (core.py, 911); _validate_rsl (core.py, 1123); validate_only_when_complete (validation_utils.py, 122); check_recursively (precheck.py, 949); SurfaceProperties (surface.py, 159); validate_rsl_zd_range (surface.py, 844)</t>
         </is>
       </c>
       <c r="D763" t="inlineStr">
@@ -22028,7 +22224,11 @@
           <t>land_cover.water.soilstorecap</t>
         </is>
       </c>
-      <c r="B766" t="inlineStr"/>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
       <c r="C766" t="inlineStr">
         <is>
           <t>SurfaceProperties (surface.py, 159); BuildingLayer (surface.py, 637)</t>
@@ -22052,7 +22252,11 @@
           <t>land_cover.water.statelimit</t>
         </is>
       </c>
-      <c r="B767" t="inlineStr"/>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
       <c r="C767" t="inlineStr">
         <is>
           <t>SurfaceProperties (surface.py, 159); BuildingLayer (surface.py, 637)</t>
@@ -22271,7 +22475,7 @@
       <c r="B776" t="inlineStr"/>
       <c r="C776" t="inlineStr">
         <is>
-          <t>SUEWSConfig (core.py, 94); _check_thermal_layers (core.py, 770); _validate_storage (core.py, 1144); YAMLAnnotator (yaml_annotator.py, 32); ValidationIssue (yaml_annotator_json.py, 16); ThermalLayers (surface.py, 25)</t>
+          <t>SUEWSConfig (core.py, 94); _check_thermal_layers (core.py, 792); _validate_storage (core.py, 1166); YAMLAnnotator (yaml_annotator.py, 32); ValidationIssue (yaml_annotator_json.py, 16); ThermalLayers (surface.py, 25)</t>
         </is>
       </c>
       <c r="D776" t="inlineStr">
@@ -24687,7 +24891,7 @@
       <c r="B866" t="inlineStr"/>
       <c r="C866" t="inlineStr">
         <is>
-          <t>_validate_stebbs (core.py, 967); StebbsProperties (site.py, 1462)</t>
+          <t>_validate_stebbs (core.py, 989); StebbsProperties (site.py, 1462)</t>
         </is>
       </c>
       <c r="D866" t="inlineStr">
@@ -24711,7 +24915,7 @@
       <c r="B867" t="inlineStr"/>
       <c r="C867" t="inlineStr">
         <is>
-          <t>_validate_stebbs (core.py, 967); StebbsProperties (site.py, 1462)</t>
+          <t>_validate_stebbs (core.py, 989); StebbsProperties (site.py, 1462)</t>
         </is>
       </c>
       <c r="D867" t="inlineStr">
@@ -24735,7 +24939,7 @@
       <c r="B868" t="inlineStr"/>
       <c r="C868" t="inlineStr">
         <is>
-          <t>_validate_stebbs (core.py, 967); StebbsProperties (site.py, 1462)</t>
+          <t>_validate_stebbs (core.py, 989); StebbsProperties (site.py, 1462)</t>
         </is>
       </c>
       <c r="D868" t="inlineStr">
@@ -24759,7 +24963,7 @@
       <c r="B869" t="inlineStr"/>
       <c r="C869" t="inlineStr">
         <is>
-          <t>_validate_stebbs (core.py, 967); StebbsProperties (site.py, 1462)</t>
+          <t>_validate_stebbs (core.py, 989); StebbsProperties (site.py, 1462)</t>
         </is>
       </c>
       <c r="D869" t="inlineStr">
@@ -24783,7 +24987,7 @@
       <c r="B870" t="inlineStr"/>
       <c r="C870" t="inlineStr">
         <is>
-          <t>_validate_stebbs (core.py, 967); StebbsProperties (site.py, 1462)</t>
+          <t>_validate_stebbs (core.py, 989); StebbsProperties (site.py, 1462)</t>
         </is>
       </c>
       <c r="D870" t="inlineStr">
@@ -24807,7 +25011,7 @@
       <c r="B871" t="inlineStr"/>
       <c r="C871" t="inlineStr">
         <is>
-          <t>_validate_stebbs (core.py, 967); StebbsProperties (site.py, 1462)</t>
+          <t>_validate_stebbs (core.py, 989); StebbsProperties (site.py, 1462)</t>
         </is>
       </c>
       <c r="D871" t="inlineStr">
@@ -24831,7 +25035,7 @@
       <c r="B872" t="inlineStr"/>
       <c r="C872" t="inlineStr">
         <is>
-          <t>_validate_stebbs (core.py, 967); StebbsProperties (site.py, 1462)</t>
+          <t>_validate_stebbs (core.py, 989); StebbsProperties (site.py, 1462)</t>
         </is>
       </c>
       <c r="D872" t="inlineStr">
@@ -24855,7 +25059,7 @@
       <c r="B873" t="inlineStr"/>
       <c r="C873" t="inlineStr">
         <is>
-          <t>_validate_stebbs (core.py, 967); StebbsProperties (site.py, 1462)</t>
+          <t>_validate_stebbs (core.py, 989); StebbsProperties (site.py, 1462)</t>
         </is>
       </c>
       <c r="D873" t="inlineStr">
@@ -24879,7 +25083,7 @@
       <c r="B874" t="inlineStr"/>
       <c r="C874" t="inlineStr">
         <is>
-          <t>_validate_stebbs (core.py, 967); StebbsProperties (site.py, 1462)</t>
+          <t>_validate_stebbs (core.py, 989); StebbsProperties (site.py, 1462)</t>
         </is>
       </c>
       <c r="D874" t="inlineStr">
@@ -24903,7 +25107,7 @@
       <c r="B875" t="inlineStr"/>
       <c r="C875" t="inlineStr">
         <is>
-          <t>_validate_stebbs (core.py, 967); StebbsProperties (site.py, 1462)</t>
+          <t>_validate_stebbs (core.py, 989); StebbsProperties (site.py, 1462)</t>
         </is>
       </c>
       <c r="D875" t="inlineStr">
@@ -24927,7 +25131,7 @@
       <c r="B876" t="inlineStr"/>
       <c r="C876" t="inlineStr">
         <is>
-          <t>_validate_stebbs (core.py, 967); StebbsProperties (site.py, 1462)</t>
+          <t>_validate_stebbs (core.py, 989); StebbsProperties (site.py, 1462)</t>
         </is>
       </c>
       <c r="D876" t="inlineStr">
@@ -24951,7 +25155,7 @@
       <c r="B877" t="inlineStr"/>
       <c r="C877" t="inlineStr">
         <is>
-          <t>_validate_stebbs (core.py, 967); StebbsProperties (site.py, 1462)</t>
+          <t>_validate_stebbs (core.py, 989); StebbsProperties (site.py, 1462)</t>
         </is>
       </c>
       <c r="D877" t="inlineStr">
@@ -24975,7 +25179,7 @@
       <c r="B878" t="inlineStr"/>
       <c r="C878" t="inlineStr">
         <is>
-          <t>_validate_stebbs (core.py, 967); StebbsProperties (site.py, 1462)</t>
+          <t>_validate_stebbs (core.py, 989); StebbsProperties (site.py, 1462)</t>
         </is>
       </c>
       <c r="D878" t="inlineStr">
@@ -24999,7 +25203,7 @@
       <c r="B879" t="inlineStr"/>
       <c r="C879" t="inlineStr">
         <is>
-          <t>_validate_stebbs (core.py, 967); StebbsProperties (site.py, 1462)</t>
+          <t>_validate_stebbs (core.py, 989); StebbsProperties (site.py, 1462)</t>
         </is>
       </c>
       <c r="D879" t="inlineStr">
@@ -25023,7 +25227,7 @@
       <c r="B880" t="inlineStr"/>
       <c r="C880" t="inlineStr">
         <is>
-          <t>_validate_stebbs (core.py, 967); StebbsProperties (site.py, 1462)</t>
+          <t>_validate_stebbs (core.py, 989); StebbsProperties (site.py, 1462)</t>
         </is>
       </c>
       <c r="D880" t="inlineStr">
@@ -25047,7 +25251,7 @@
       <c r="B881" t="inlineStr"/>
       <c r="C881" t="inlineStr">
         <is>
-          <t>_validate_stebbs (core.py, 967); StebbsProperties (site.py, 1462)</t>
+          <t>_validate_stebbs (core.py, 989); StebbsProperties (site.py, 1462)</t>
         </is>
       </c>
       <c r="D881" t="inlineStr">
@@ -25071,7 +25275,7 @@
       <c r="B882" t="inlineStr"/>
       <c r="C882" t="inlineStr">
         <is>
-          <t>_validate_stebbs (core.py, 967); StebbsProperties (site.py, 1462)</t>
+          <t>_validate_stebbs (core.py, 989); StebbsProperties (site.py, 1462)</t>
         </is>
       </c>
       <c r="D882" t="inlineStr">
@@ -25095,7 +25299,7 @@
       <c r="B883" t="inlineStr"/>
       <c r="C883" t="inlineStr">
         <is>
-          <t>_validate_stebbs (core.py, 967); StebbsProperties (site.py, 1462)</t>
+          <t>_validate_stebbs (core.py, 989); StebbsProperties (site.py, 1462)</t>
         </is>
       </c>
       <c r="D883" t="inlineStr">
@@ -25119,7 +25323,7 @@
       <c r="B884" t="inlineStr"/>
       <c r="C884" t="inlineStr">
         <is>
-          <t>_validate_stebbs (core.py, 967); StebbsProperties (site.py, 1462)</t>
+          <t>_validate_stebbs (core.py, 989); StebbsProperties (site.py, 1462)</t>
         </is>
       </c>
       <c r="D884" t="inlineStr">
@@ -25143,7 +25347,7 @@
       <c r="B885" t="inlineStr"/>
       <c r="C885" t="inlineStr">
         <is>
-          <t>_validate_stebbs (core.py, 967); StebbsProperties (site.py, 1462)</t>
+          <t>_validate_stebbs (core.py, 989); StebbsProperties (site.py, 1462)</t>
         </is>
       </c>
       <c r="D885" t="inlineStr">
@@ -25167,7 +25371,7 @@
       <c r="B886" t="inlineStr"/>
       <c r="C886" t="inlineStr">
         <is>
-          <t>_validate_stebbs (core.py, 967); StebbsProperties (site.py, 1462)</t>
+          <t>_validate_stebbs (core.py, 989); StebbsProperties (site.py, 1462)</t>
         </is>
       </c>
       <c r="D886" t="inlineStr">
@@ -25188,10 +25392,14 @@
           <t>stebbs.GroundDepth</t>
         </is>
       </c>
-      <c r="B887" t="inlineStr"/>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
       <c r="C887" t="inlineStr">
         <is>
-          <t>_validate_stebbs (core.py, 967); StebbsProperties (site.py, 1462)</t>
+          <t>_validate_stebbs (core.py, 989); StebbsProperties (site.py, 1462)</t>
         </is>
       </c>
       <c r="D887" t="inlineStr">
@@ -25215,7 +25423,7 @@
       <c r="B888" t="inlineStr"/>
       <c r="C888" t="inlineStr">
         <is>
-          <t>_validate_stebbs (core.py, 967); StebbsProperties (site.py, 1462)</t>
+          <t>_validate_stebbs (core.py, 989); StebbsProperties (site.py, 1462)</t>
         </is>
       </c>
       <c r="D888" t="inlineStr">
@@ -25239,7 +25447,7 @@
       <c r="B889" t="inlineStr"/>
       <c r="C889" t="inlineStr">
         <is>
-          <t>_validate_stebbs (core.py, 967); StebbsProperties (site.py, 1462)</t>
+          <t>_validate_stebbs (core.py, 989); StebbsProperties (site.py, 1462)</t>
         </is>
       </c>
       <c r="D889" t="inlineStr">
@@ -25263,7 +25471,7 @@
       <c r="B890" t="inlineStr"/>
       <c r="C890" t="inlineStr">
         <is>
-          <t>_validate_stebbs (core.py, 967); StebbsProperties (site.py, 1462)</t>
+          <t>_validate_stebbs (core.py, 989); StebbsProperties (site.py, 1462)</t>
         </is>
       </c>
       <c r="D890" t="inlineStr">
@@ -25287,7 +25495,7 @@
       <c r="B891" t="inlineStr"/>
       <c r="C891" t="inlineStr">
         <is>
-          <t>_validate_stebbs (core.py, 967); StebbsProperties (site.py, 1462)</t>
+          <t>_validate_stebbs (core.py, 989); StebbsProperties (site.py, 1462)</t>
         </is>
       </c>
       <c r="D891" t="inlineStr">
@@ -25311,7 +25519,7 @@
       <c r="B892" t="inlineStr"/>
       <c r="C892" t="inlineStr">
         <is>
-          <t>_validate_stebbs (core.py, 967); StebbsProperties (site.py, 1462)</t>
+          <t>_validate_stebbs (core.py, 989); StebbsProperties (site.py, 1462)</t>
         </is>
       </c>
       <c r="D892" t="inlineStr">
@@ -25335,7 +25543,7 @@
       <c r="B893" t="inlineStr"/>
       <c r="C893" t="inlineStr">
         <is>
-          <t>_validate_stebbs (core.py, 967); StebbsProperties (site.py, 1462)</t>
+          <t>_validate_stebbs (core.py, 989); StebbsProperties (site.py, 1462)</t>
         </is>
       </c>
       <c r="D893" t="inlineStr">
@@ -25359,7 +25567,7 @@
       <c r="B894" t="inlineStr"/>
       <c r="C894" t="inlineStr">
         <is>
-          <t>_validate_stebbs (core.py, 967); StebbsProperties (site.py, 1462)</t>
+          <t>_validate_stebbs (core.py, 989); StebbsProperties (site.py, 1462)</t>
         </is>
       </c>
       <c r="D894" t="inlineStr">
@@ -25383,7 +25591,7 @@
       <c r="B895" t="inlineStr"/>
       <c r="C895" t="inlineStr">
         <is>
-          <t>_validate_stebbs (core.py, 967); StebbsProperties (site.py, 1462)</t>
+          <t>_validate_stebbs (core.py, 989); StebbsProperties (site.py, 1462)</t>
         </is>
       </c>
       <c r="D895" t="inlineStr">
@@ -25407,7 +25615,7 @@
       <c r="B896" t="inlineStr"/>
       <c r="C896" t="inlineStr">
         <is>
-          <t>_validate_stebbs (core.py, 967); StebbsProperties (site.py, 1462)</t>
+          <t>_validate_stebbs (core.py, 989); StebbsProperties (site.py, 1462)</t>
         </is>
       </c>
       <c r="D896" t="inlineStr">
@@ -25431,7 +25639,7 @@
       <c r="B897" t="inlineStr"/>
       <c r="C897" t="inlineStr">
         <is>
-          <t>_validate_stebbs (core.py, 967); StebbsProperties (site.py, 1462)</t>
+          <t>_validate_stebbs (core.py, 989); StebbsProperties (site.py, 1462)</t>
         </is>
       </c>
       <c r="D897" t="inlineStr">
@@ -25455,7 +25663,7 @@
       <c r="B898" t="inlineStr"/>
       <c r="C898" t="inlineStr">
         <is>
-          <t>_validate_stebbs (core.py, 967); StebbsProperties (site.py, 1462)</t>
+          <t>_validate_stebbs (core.py, 989); StebbsProperties (site.py, 1462)</t>
         </is>
       </c>
       <c r="D898" t="inlineStr">
@@ -25479,7 +25687,7 @@
       <c r="B899" t="inlineStr"/>
       <c r="C899" t="inlineStr">
         <is>
-          <t>_validate_stebbs (core.py, 967); StebbsProperties (site.py, 1462)</t>
+          <t>_validate_stebbs (core.py, 989); StebbsProperties (site.py, 1462)</t>
         </is>
       </c>
       <c r="D899" t="inlineStr">
@@ -25503,7 +25711,7 @@
       <c r="B900" t="inlineStr"/>
       <c r="C900" t="inlineStr">
         <is>
-          <t>_validate_stebbs (core.py, 967); StebbsProperties (site.py, 1462)</t>
+          <t>_validate_stebbs (core.py, 989); StebbsProperties (site.py, 1462)</t>
         </is>
       </c>
       <c r="D900" t="inlineStr">
@@ -25527,7 +25735,7 @@
       <c r="B901" t="inlineStr"/>
       <c r="C901" t="inlineStr">
         <is>
-          <t>_validate_stebbs (core.py, 967); StebbsProperties (site.py, 1462)</t>
+          <t>_validate_stebbs (core.py, 989); StebbsProperties (site.py, 1462)</t>
         </is>
       </c>
       <c r="D901" t="inlineStr">
@@ -25551,7 +25759,7 @@
       <c r="B902" t="inlineStr"/>
       <c r="C902" t="inlineStr">
         <is>
-          <t>_validate_stebbs (core.py, 967); StebbsProperties (site.py, 1462)</t>
+          <t>_validate_stebbs (core.py, 989); StebbsProperties (site.py, 1462)</t>
         </is>
       </c>
       <c r="D902" t="inlineStr">
@@ -25575,7 +25783,7 @@
       <c r="B903" t="inlineStr"/>
       <c r="C903" t="inlineStr">
         <is>
-          <t>_validate_stebbs (core.py, 967); StebbsProperties (site.py, 1462)</t>
+          <t>_validate_stebbs (core.py, 989); StebbsProperties (site.py, 1462)</t>
         </is>
       </c>
       <c r="D903" t="inlineStr">
@@ -25599,7 +25807,7 @@
       <c r="B904" t="inlineStr"/>
       <c r="C904" t="inlineStr">
         <is>
-          <t>_validate_stebbs (core.py, 967); StebbsProperties (site.py, 1462)</t>
+          <t>_validate_stebbs (core.py, 989); StebbsProperties (site.py, 1462)</t>
         </is>
       </c>
       <c r="D904" t="inlineStr">
@@ -25623,7 +25831,7 @@
       <c r="B905" t="inlineStr"/>
       <c r="C905" t="inlineStr">
         <is>
-          <t>_validate_stebbs (core.py, 967); StebbsProperties (site.py, 1462)</t>
+          <t>_validate_stebbs (core.py, 989); StebbsProperties (site.py, 1462)</t>
         </is>
       </c>
       <c r="D905" t="inlineStr">
@@ -25647,7 +25855,7 @@
       <c r="B906" t="inlineStr"/>
       <c r="C906" t="inlineStr">
         <is>
-          <t>_validate_stebbs (core.py, 967); StebbsProperties (site.py, 1462)</t>
+          <t>_validate_stebbs (core.py, 989); StebbsProperties (site.py, 1462)</t>
         </is>
       </c>
       <c r="D906" t="inlineStr">
@@ -25671,7 +25879,7 @@
       <c r="B907" t="inlineStr"/>
       <c r="C907" t="inlineStr">
         <is>
-          <t>_validate_stebbs (core.py, 967); StebbsProperties (site.py, 1462)</t>
+          <t>_validate_stebbs (core.py, 989); StebbsProperties (site.py, 1462)</t>
         </is>
       </c>
       <c r="D907" t="inlineStr">
@@ -25695,7 +25903,7 @@
       <c r="B908" t="inlineStr"/>
       <c r="C908" t="inlineStr">
         <is>
-          <t>_validate_stebbs (core.py, 967); StebbsProperties (site.py, 1462)</t>
+          <t>_validate_stebbs (core.py, 989); StebbsProperties (site.py, 1462)</t>
         </is>
       </c>
       <c r="D908" t="inlineStr">
@@ -25719,7 +25927,7 @@
       <c r="B909" t="inlineStr"/>
       <c r="C909" t="inlineStr">
         <is>
-          <t>_validate_stebbs (core.py, 967); StebbsProperties (site.py, 1462)</t>
+          <t>_validate_stebbs (core.py, 989); StebbsProperties (site.py, 1462)</t>
         </is>
       </c>
       <c r="D909" t="inlineStr">
@@ -25743,7 +25951,7 @@
       <c r="B910" t="inlineStr"/>
       <c r="C910" t="inlineStr">
         <is>
-          <t>_validate_stebbs (core.py, 967); StebbsProperties (site.py, 1462)</t>
+          <t>_validate_stebbs (core.py, 989); StebbsProperties (site.py, 1462)</t>
         </is>
       </c>
       <c r="D910" t="inlineStr">
@@ -25767,7 +25975,7 @@
       <c r="B911" t="inlineStr"/>
       <c r="C911" t="inlineStr">
         <is>
-          <t>_validate_stebbs (core.py, 967); StebbsProperties (site.py, 1462)</t>
+          <t>_validate_stebbs (core.py, 989); StebbsProperties (site.py, 1462)</t>
         </is>
       </c>
       <c r="D911" t="inlineStr">
@@ -25791,7 +25999,7 @@
       <c r="B912" t="inlineStr"/>
       <c r="C912" t="inlineStr">
         <is>
-          <t>_validate_stebbs (core.py, 967); StebbsProperties (site.py, 1462)</t>
+          <t>_validate_stebbs (core.py, 989); StebbsProperties (site.py, 1462)</t>
         </is>
       </c>
       <c r="D912" t="inlineStr">
@@ -25815,7 +26023,7 @@
       <c r="B913" t="inlineStr"/>
       <c r="C913" t="inlineStr">
         <is>
-          <t>_validate_stebbs (core.py, 967); StebbsProperties (site.py, 1462)</t>
+          <t>_validate_stebbs (core.py, 989); StebbsProperties (site.py, 1462)</t>
         </is>
       </c>
       <c r="D913" t="inlineStr">
@@ -25839,7 +26047,7 @@
       <c r="B914" t="inlineStr"/>
       <c r="C914" t="inlineStr">
         <is>
-          <t>_validate_stebbs (core.py, 967); StebbsProperties (site.py, 1462)</t>
+          <t>_validate_stebbs (core.py, 989); StebbsProperties (site.py, 1462)</t>
         </is>
       </c>
       <c r="D914" t="inlineStr">
@@ -25863,7 +26071,7 @@
       <c r="B915" t="inlineStr"/>
       <c r="C915" t="inlineStr">
         <is>
-          <t>_validate_stebbs (core.py, 967); StebbsProperties (site.py, 1462)</t>
+          <t>_validate_stebbs (core.py, 989); StebbsProperties (site.py, 1462)</t>
         </is>
       </c>
       <c r="D915" t="inlineStr">
@@ -25887,7 +26095,7 @@
       <c r="B916" t="inlineStr"/>
       <c r="C916" t="inlineStr">
         <is>
-          <t>_validate_stebbs (core.py, 967); StebbsProperties (site.py, 1462)</t>
+          <t>_validate_stebbs (core.py, 989); StebbsProperties (site.py, 1462)</t>
         </is>
       </c>
       <c r="D916" t="inlineStr">
@@ -25911,7 +26119,7 @@
       <c r="B917" t="inlineStr"/>
       <c r="C917" t="inlineStr">
         <is>
-          <t>_validate_stebbs (core.py, 967); StebbsProperties (site.py, 1462)</t>
+          <t>_validate_stebbs (core.py, 989); StebbsProperties (site.py, 1462)</t>
         </is>
       </c>
       <c r="D917" t="inlineStr">
@@ -25935,7 +26143,7 @@
       <c r="B918" t="inlineStr"/>
       <c r="C918" t="inlineStr">
         <is>
-          <t>_validate_stebbs (core.py, 967); StebbsProperties (site.py, 1462)</t>
+          <t>_validate_stebbs (core.py, 989); StebbsProperties (site.py, 1462)</t>
         </is>
       </c>
       <c r="D918" t="inlineStr">
@@ -25959,7 +26167,7 @@
       <c r="B919" t="inlineStr"/>
       <c r="C919" t="inlineStr">
         <is>
-          <t>_validate_stebbs (core.py, 967); StebbsProperties (site.py, 1462)</t>
+          <t>_validate_stebbs (core.py, 989); StebbsProperties (site.py, 1462)</t>
         </is>
       </c>
       <c r="D919" t="inlineStr">
@@ -25983,7 +26191,7 @@
       <c r="B920" t="inlineStr"/>
       <c r="C920" t="inlineStr">
         <is>
-          <t>_validate_stebbs (core.py, 967); StebbsProperties (site.py, 1462)</t>
+          <t>_validate_stebbs (core.py, 989); StebbsProperties (site.py, 1462)</t>
         </is>
       </c>
       <c r="D920" t="inlineStr">
@@ -26007,7 +26215,7 @@
       <c r="B921" t="inlineStr"/>
       <c r="C921" t="inlineStr">
         <is>
-          <t>_validate_stebbs (core.py, 967); StebbsProperties (site.py, 1462)</t>
+          <t>_validate_stebbs (core.py, 989); StebbsProperties (site.py, 1462)</t>
         </is>
       </c>
       <c r="D921" t="inlineStr">
@@ -26031,7 +26239,7 @@
       <c r="B922" t="inlineStr"/>
       <c r="C922" t="inlineStr">
         <is>
-          <t>_validate_stebbs (core.py, 967); StebbsProperties (site.py, 1462)</t>
+          <t>_validate_stebbs (core.py, 989); StebbsProperties (site.py, 1462)</t>
         </is>
       </c>
       <c r="D922" t="inlineStr">
@@ -26055,7 +26263,7 @@
       <c r="B923" t="inlineStr"/>
       <c r="C923" t="inlineStr">
         <is>
-          <t>_validate_stebbs (core.py, 967); StebbsProperties (site.py, 1462)</t>
+          <t>_validate_stebbs (core.py, 989); StebbsProperties (site.py, 1462)</t>
         </is>
       </c>
       <c r="D923" t="inlineStr">
@@ -26079,7 +26287,7 @@
       <c r="B924" t="inlineStr"/>
       <c r="C924" t="inlineStr">
         <is>
-          <t>_validate_stebbs (core.py, 967); StebbsProperties (site.py, 1462)</t>
+          <t>_validate_stebbs (core.py, 989); StebbsProperties (site.py, 1462)</t>
         </is>
       </c>
       <c r="D924" t="inlineStr">
@@ -26103,7 +26311,7 @@
       <c r="B925" t="inlineStr"/>
       <c r="C925" t="inlineStr">
         <is>
-          <t>_validate_stebbs (core.py, 967); StebbsProperties (site.py, 1462)</t>
+          <t>_validate_stebbs (core.py, 989); StebbsProperties (site.py, 1462)</t>
         </is>
       </c>
       <c r="D925" t="inlineStr">
@@ -26127,7 +26335,7 @@
       <c r="B926" t="inlineStr"/>
       <c r="C926" t="inlineStr">
         <is>
-          <t>_validate_stebbs (core.py, 967); StebbsProperties (site.py, 1462)</t>
+          <t>_validate_stebbs (core.py, 989); StebbsProperties (site.py, 1462)</t>
         </is>
       </c>
       <c r="D926" t="inlineStr">
@@ -26151,7 +26359,7 @@
       <c r="B927" t="inlineStr"/>
       <c r="C927" t="inlineStr">
         <is>
-          <t>_validate_stebbs (core.py, 967); StebbsProperties (site.py, 1462)</t>
+          <t>_validate_stebbs (core.py, 989); StebbsProperties (site.py, 1462)</t>
         </is>
       </c>
       <c r="D927" t="inlineStr">
@@ -26175,7 +26383,7 @@
       <c r="B928" t="inlineStr"/>
       <c r="C928" t="inlineStr">
         <is>
-          <t>_validate_stebbs (core.py, 967); StebbsProperties (site.py, 1462)</t>
+          <t>_validate_stebbs (core.py, 989); StebbsProperties (site.py, 1462)</t>
         </is>
       </c>
       <c r="D928" t="inlineStr">
@@ -26199,7 +26407,7 @@
       <c r="B929" t="inlineStr"/>
       <c r="C929" t="inlineStr">
         <is>
-          <t>_validate_stebbs (core.py, 967); StebbsProperties (site.py, 1462)</t>
+          <t>_validate_stebbs (core.py, 989); StebbsProperties (site.py, 1462)</t>
         </is>
       </c>
       <c r="D929" t="inlineStr">
@@ -26271,7 +26479,7 @@
       <c r="B932" t="inlineStr"/>
       <c r="C932" t="inlineStr">
         <is>
-          <t>validate_building_layers (core.py, 1533); VerticalLayers (surface.py, 976)</t>
+          <t>validate_building_layers (core.py, 1569); VerticalLayers (surface.py, 976)</t>
         </is>
       </c>
       <c r="D932" t="inlineStr">
@@ -26295,7 +26503,7 @@
       <c r="B933" t="inlineStr"/>
       <c r="C933" t="inlineStr">
         <is>
-          <t>validate_building_layers (core.py, 1533); VerticalLayers (surface.py, 976)</t>
+          <t>validate_building_layers (core.py, 1569); VerticalLayers (surface.py, 976)</t>
         </is>
       </c>
       <c r="D933" t="inlineStr">
@@ -26319,7 +26527,7 @@
       <c r="B934" t="inlineStr"/>
       <c r="C934" t="inlineStr">
         <is>
-          <t>_check_surface_parameters (core.py, 710); validate_building_layers (core.py, 1533); _validate_rst_parameters (validation_controller.py, 215); _validate_variable_roughness_parameters (validation_controller.py, 266); VerticalLayers (surface.py, 976); validate_rsl_zd_range (surface.py, 844)</t>
+          <t>_check_surface_parameters (core.py, 732); validate_building_layers (core.py, 1569); _validate_rst_parameters (validation_controller.py, 215); _validate_variable_roughness_parameters (validation_controller.py, 266); VerticalLayers (surface.py, 976); validate_rsl_zd_range (surface.py, 844)</t>
         </is>
       </c>
       <c r="D934" t="inlineStr">
@@ -26343,7 +26551,7 @@
       <c r="B935" t="inlineStr"/>
       <c r="C935" t="inlineStr">
         <is>
-          <t>validate_building_layers (core.py, 1533); VerticalLayers (surface.py, 976)</t>
+          <t>validate_building_layers (core.py, 1569); VerticalLayers (surface.py, 976)</t>
         </is>
       </c>
       <c r="D935" t="inlineStr">
@@ -26367,7 +26575,7 @@
       <c r="B936" t="inlineStr"/>
       <c r="C936" t="inlineStr">
         <is>
-          <t>SUEWSConfig (core.py, 94); validate_building_layers (core.py, 1533); VerticalLayers (surface.py, 976); InitialStates (state.py, 761)</t>
+          <t>SUEWSConfig (core.py, 94); validate_building_layers (core.py, 1569); VerticalLayers (surface.py, 976); InitialStates (state.py, 761)</t>
         </is>
       </c>
       <c r="D936" t="inlineStr">
@@ -26439,7 +26647,7 @@
       <c r="B939" t="inlineStr"/>
       <c r="C939" t="inlineStr">
         <is>
-          <t>SUEWSConfig (core.py, 94); _validate_storage (core.py, 1144); validate_building_layers (core.py, 1533); VerticalLayers (surface.py, 976); InitialStates (state.py, 761)</t>
+          <t>SUEWSConfig (core.py, 94); _validate_storage (core.py, 1166); validate_building_layers (core.py, 1569); VerticalLayers (surface.py, 976); InitialStates (state.py, 761)</t>
         </is>
       </c>
       <c r="D939" t="inlineStr">

</xml_diff>